<commit_message>
Completed Draft Bill except for container rows
</commit_message>
<xml_diff>
--- a/AmbRcnTradeServer/ExcelTemplates/Maersk Draft BL Template BL.xlsx
+++ b/AmbRcnTradeServer/ExcelTemplates/Maersk Draft BL Template BL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Visual Studio\AmbRcnTrade\AmbRcnTradeServer\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16925FB-9B53-4D25-8E2C-51609CD7A500}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6961EFDF-C8AD-4A5C-87DE-0E722F247783}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="10680" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="103">
   <si>
     <t>Shipping Instruction submitter (who should Safmarine Line contact in case of  any queries to this document)</t>
   </si>
@@ -253,9 +253,6 @@
     <t>BillLading.ConsigneeAddress5</t>
   </si>
   <si>
-    <t>BillLading.DestinationAgentAddress</t>
-  </si>
-  <si>
     <t>BillLading.NotifyParty1CompanyName</t>
   </si>
   <si>
@@ -314,13 +311,38 @@
   </si>
   <si>
     <t>BillLading.FreightDestinationChargePaidBy</t>
+  </si>
+  <si>
+    <t>BillLading.CargoDescription</t>
+  </si>
+  <si>
+    <t>BillLading.ShippingMarks</t>
+  </si>
+  <si>
+    <t>BillLading.NumberPackagesText</t>
+  </si>
+  <si>
+    <t>BillLading.GrossWeightKgText</t>
+  </si>
+  <si>
+    <t>BillLading.VgmWeightKgText
+(Kgs)*</t>
+  </si>
+  <si>
+    <t>BillLading.DestinationAgentCompanyName</t>
+  </si>
+  <si>
+    <t>BillLading.PreCargoDescription.Header</t>
+  </si>
+  <si>
+    <t>BillLading.PreCargoDescription.Footer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,13 +354,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -849,7 +864,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -875,11 +890,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -888,15 +899,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -908,8 +919,248 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -965,26 +1216,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -995,240 +1234,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -1236,7 +1273,245 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="51">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1692,8 +1967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56:L56"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -1729,79 +2004,79 @@
     </row>
     <row r="2" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="37"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="106"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="40"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="107"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="108"/>
+      <c r="J3" s="108"/>
+      <c r="K3" s="108"/>
+      <c r="L3" s="109"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="40"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="107"/>
+      <c r="H4" s="108"/>
+      <c r="I4" s="108"/>
+      <c r="J4" s="108"/>
+      <c r="K4" s="108"/>
+      <c r="L4" s="109"/>
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="43"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="103"/>
+      <c r="G5" s="110"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="111"/>
+      <c r="J5" s="111"/>
+      <c r="K5" s="111"/>
+      <c r="L5" s="112"/>
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1"/>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="46"/>
+      <c r="C6" s="114"/>
+      <c r="D6" s="114"/>
+      <c r="E6" s="114"/>
+      <c r="F6" s="114"/>
+      <c r="G6" s="114"/>
+      <c r="H6" s="114"/>
+      <c r="I6" s="114"/>
+      <c r="J6" s="114"/>
+      <c r="K6" s="114"/>
+      <c r="L6" s="115"/>
       <c r="M6" s="1"/>
       <c r="N6" s="2"/>
     </row>
@@ -1810,20 +2085,20 @@
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="49"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="91"/>
       <c r="G7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="50"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="52"/>
+      <c r="H7" s="116"/>
+      <c r="I7" s="117"/>
+      <c r="J7" s="117"/>
+      <c r="K7" s="117"/>
+      <c r="L7" s="118"/>
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1831,18 +2106,18 @@
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="49"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
+      <c r="L8" s="91"/>
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1850,424 +2125,424 @@
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="49"/>
+      <c r="D9" s="90"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="91"/>
       <c r="G9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="47">
+      <c r="H9" s="89">
         <v>3</v>
       </c>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="49"/>
+      <c r="I9" s="90"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="91"/>
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="1"/>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="56" t="s">
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="58"/>
+      <c r="H10" s="93"/>
+      <c r="I10" s="93"/>
+      <c r="J10" s="93"/>
+      <c r="K10" s="93"/>
+      <c r="L10" s="94"/>
       <c r="M10" s="6"/>
       <c r="N10" s="7"/>
     </row>
     <row r="11" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
-      <c r="B11" s="59" t="s">
+      <c r="B11" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="61"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="70"/>
       <c r="G11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="62" t="s">
+      <c r="H11" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="I11" s="63"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="63"/>
-      <c r="L11" s="64"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="86"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="87"/>
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
-      <c r="B12" s="65" t="s">
+      <c r="B12" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="67"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="64"/>
       <c r="G12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="68" t="s">
+      <c r="H12" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="I12" s="69"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="70"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="88"/>
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
-      <c r="B13" s="65" t="s">
+      <c r="B13" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="67"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="64"/>
       <c r="G13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="68" t="s">
+      <c r="H13" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="I13" s="69"/>
-      <c r="J13" s="69"/>
-      <c r="K13" s="69"/>
-      <c r="L13" s="70"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="88"/>
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
-      <c r="B14" s="65" t="s">
+      <c r="B14" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="71" t="s">
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="72"/>
-      <c r="I14" s="72"/>
-      <c r="J14" s="72"/>
-      <c r="K14" s="72"/>
-      <c r="L14" s="73"/>
+      <c r="H14" s="75"/>
+      <c r="I14" s="75"/>
+      <c r="J14" s="75"/>
+      <c r="K14" s="75"/>
+      <c r="L14" s="76"/>
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
-      <c r="B15" s="65" t="s">
+      <c r="B15" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="66"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="74"/>
-      <c r="H15" s="75"/>
-      <c r="I15" s="75"/>
-      <c r="J15" s="75"/>
-      <c r="K15" s="75"/>
-      <c r="L15" s="76"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="77"/>
+      <c r="H15" s="78"/>
+      <c r="I15" s="78"/>
+      <c r="J15" s="78"/>
+      <c r="K15" s="78"/>
+      <c r="L15" s="79"/>
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="1"/>
-      <c r="B16" s="65" t="s">
+      <c r="B16" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="77"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="78"/>
-      <c r="J16" s="78"/>
-      <c r="K16" s="78"/>
-      <c r="L16" s="79"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="81"/>
+      <c r="I16" s="81"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="81"/>
+      <c r="L16" s="82"/>
       <c r="M16" s="1"/>
     </row>
     <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1"/>
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="53" t="s">
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="84"/>
+      <c r="G17" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="54"/>
-      <c r="L17" s="55"/>
+      <c r="H17" s="66"/>
+      <c r="I17" s="66"/>
+      <c r="J17" s="66"/>
+      <c r="K17" s="66"/>
+      <c r="L17" s="84"/>
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="59" t="s">
-        <v>84</v>
-      </c>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="60"/>
-      <c r="L18" s="61"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="69"/>
+      <c r="K18" s="69"/>
+      <c r="L18" s="70"/>
       <c r="M18" s="1"/>
     </row>
     <row r="19" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
-      <c r="B19" s="80" t="s">
+      <c r="B19" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
-      <c r="E19" s="81"/>
-      <c r="F19" s="82"/>
-      <c r="G19" s="65" t="s">
+      <c r="C19" s="72"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="H19" s="66"/>
-      <c r="I19" s="66"/>
-      <c r="J19" s="66"/>
-      <c r="K19" s="66"/>
-      <c r="L19" s="67"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="44"/>
+      <c r="L19" s="64"/>
       <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
-      <c r="B20" s="80" t="s">
+      <c r="B20" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
-      <c r="E20" s="81"/>
-      <c r="F20" s="82"/>
-      <c r="G20" s="65" t="s">
+      <c r="C20" s="72"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="H20" s="66"/>
-      <c r="I20" s="66"/>
-      <c r="J20" s="66"/>
-      <c r="K20" s="66"/>
-      <c r="L20" s="67"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="64"/>
       <c r="M20" s="1"/>
     </row>
     <row r="21" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
-      <c r="B21" s="80" t="s">
+      <c r="B21" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="81"/>
-      <c r="F21" s="82"/>
-      <c r="G21" s="65" t="s">
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="66"/>
-      <c r="I21" s="66"/>
-      <c r="J21" s="66"/>
-      <c r="K21" s="66"/>
-      <c r="L21" s="67"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="64"/>
       <c r="M21" s="1"/>
     </row>
     <row r="22" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
-      <c r="B22" s="80" t="s">
+      <c r="B22" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="81"/>
-      <c r="D22" s="81"/>
-      <c r="E22" s="81"/>
-      <c r="F22" s="82"/>
-      <c r="G22" s="65" t="s">
+      <c r="C22" s="72"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="H22" s="66"/>
-      <c r="I22" s="66"/>
-      <c r="J22" s="66"/>
-      <c r="K22" s="66"/>
-      <c r="L22" s="67"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="64"/>
       <c r="M22" s="1"/>
     </row>
     <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="1"/>
-      <c r="B23" s="80" t="s">
+      <c r="B23" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="81"/>
-      <c r="D23" s="81"/>
-      <c r="E23" s="81"/>
-      <c r="F23" s="82"/>
-      <c r="G23" s="65" t="s">
+      <c r="C23" s="72"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="H23" s="66"/>
-      <c r="I23" s="66"/>
-      <c r="J23" s="66"/>
-      <c r="K23" s="66"/>
-      <c r="L23" s="67"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="64"/>
       <c r="M23" s="1"/>
     </row>
     <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="1"/>
-      <c r="B24" s="83" t="s">
+      <c r="B24" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="84"/>
-      <c r="G24" s="83" t="s">
+      <c r="C24" s="66"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="84"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="66"/>
+      <c r="J24" s="66"/>
+      <c r="K24" s="66"/>
+      <c r="L24" s="67"/>
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
-      <c r="B25" s="59" t="s">
+      <c r="B25" s="68" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="60"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="59" t="s">
-        <v>77</v>
-      </c>
-      <c r="H25" s="60"/>
-      <c r="I25" s="60"/>
-      <c r="J25" s="60"/>
-      <c r="K25" s="60"/>
-      <c r="L25" s="61"/>
+      <c r="H25" s="69"/>
+      <c r="I25" s="69"/>
+      <c r="J25" s="69"/>
+      <c r="K25" s="69"/>
+      <c r="L25" s="70"/>
       <c r="M25" s="1"/>
     </row>
     <row r="26" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
-      <c r="B26" s="65" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" s="66"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="66"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="65" t="s">
-        <v>78</v>
-      </c>
-      <c r="H26" s="66"/>
-      <c r="I26" s="66"/>
-      <c r="J26" s="66"/>
-      <c r="K26" s="66"/>
-      <c r="L26" s="67"/>
+      <c r="B26" s="63" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="64"/>
+      <c r="G26" s="63" t="s">
+        <v>77</v>
+      </c>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="64"/>
       <c r="M26" s="1"/>
     </row>
     <row r="27" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
-      <c r="B27" s="65" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" s="66"/>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="67"/>
-      <c r="G27" s="65" t="s">
-        <v>79</v>
-      </c>
-      <c r="H27" s="66"/>
-      <c r="I27" s="66"/>
-      <c r="J27" s="66"/>
-      <c r="K27" s="66"/>
-      <c r="L27" s="67"/>
+      <c r="B27" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="63" t="s">
+        <v>78</v>
+      </c>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="64"/>
       <c r="M27" s="1"/>
     </row>
     <row r="28" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
-      <c r="B28" s="65" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="66"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="66"/>
-      <c r="F28" s="67"/>
-      <c r="G28" s="65" t="s">
-        <v>80</v>
-      </c>
-      <c r="H28" s="66"/>
-      <c r="I28" s="66"/>
-      <c r="J28" s="66"/>
-      <c r="K28" s="66"/>
-      <c r="L28" s="67"/>
+      <c r="B28" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="64"/>
+      <c r="G28" s="63" t="s">
+        <v>79</v>
+      </c>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="64"/>
       <c r="M28" s="1"/>
     </row>
     <row r="29" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
-      <c r="B29" s="65" t="s">
-        <v>88</v>
-      </c>
-      <c r="C29" s="66"/>
-      <c r="D29" s="66"/>
-      <c r="E29" s="66"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="65" t="s">
-        <v>81</v>
-      </c>
-      <c r="H29" s="66"/>
-      <c r="I29" s="66"/>
-      <c r="J29" s="66"/>
-      <c r="K29" s="66"/>
-      <c r="L29" s="67"/>
+      <c r="B29" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="64"/>
+      <c r="G29" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="64"/>
       <c r="M29" s="1"/>
     </row>
     <row r="30" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
-      <c r="B30" s="65" t="s">
-        <v>89</v>
-      </c>
-      <c r="C30" s="66"/>
-      <c r="D30" s="66"/>
-      <c r="E30" s="66"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="65" t="s">
-        <v>82</v>
-      </c>
-      <c r="H30" s="66"/>
-      <c r="I30" s="66"/>
-      <c r="J30" s="66"/>
-      <c r="K30" s="66"/>
-      <c r="L30" s="67"/>
+      <c r="B30" s="63" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="64"/>
+      <c r="G30" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="64"/>
       <c r="M30" s="1"/>
     </row>
     <row r="31" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
@@ -2275,58 +2550,58 @@
       <c r="B31" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="85" t="s">
+      <c r="C31" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="66"/>
-      <c r="E31" s="66"/>
-      <c r="F31" s="86"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="45"/>
       <c r="G31" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H31" s="85" t="s">
-        <v>75</v>
-      </c>
-      <c r="I31" s="66"/>
-      <c r="J31" s="66"/>
-      <c r="K31" s="66"/>
-      <c r="L31" s="86"/>
+      <c r="H31" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="I31" s="44"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="44"/>
+      <c r="L31" s="45"/>
       <c r="M31" s="1"/>
     </row>
     <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
-      <c r="B32" s="87" t="s">
+      <c r="B32" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="88"/>
-      <c r="D32" s="88"/>
-      <c r="E32" s="88"/>
-      <c r="F32" s="89"/>
-      <c r="G32" s="90" t="s">
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="H32" s="91"/>
-      <c r="I32" s="91"/>
-      <c r="J32" s="91"/>
-      <c r="K32" s="91"/>
-      <c r="L32" s="92"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="41"/>
+      <c r="L32" s="42"/>
       <c r="M32" s="1"/>
     </row>
     <row r="33" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
-      <c r="B33" s="68"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="93"/>
-      <c r="G33" s="68" t="s">
+      <c r="B33" s="60"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="62"/>
+      <c r="G33" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="H33" s="69"/>
-      <c r="I33" s="69"/>
-      <c r="J33" s="69"/>
-      <c r="K33" s="69"/>
-      <c r="L33" s="93"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="61"/>
+      <c r="J33" s="61"/>
+      <c r="K33" s="61"/>
+      <c r="L33" s="62"/>
       <c r="M33" s="1"/>
     </row>
     <row r="34" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2334,552 +2609,558 @@
       <c r="B34" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="94" t="s">
+      <c r="C34" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="95"/>
-      <c r="E34" s="95"/>
-      <c r="F34" s="96"/>
-      <c r="G34" s="97" t="s">
+      <c r="D34" s="55"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="H34" s="98"/>
-      <c r="I34" s="98"/>
-      <c r="J34" s="98"/>
-      <c r="K34" s="98"/>
-      <c r="L34" s="99"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="58"/>
+      <c r="J34" s="58"/>
+      <c r="K34" s="58"/>
+      <c r="L34" s="59"/>
       <c r="M34" s="1"/>
     </row>
     <row r="35" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
-      <c r="B35" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C35" s="68" t="s">
+      <c r="B35" s="127" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="69"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="93"/>
-      <c r="G35" s="85"/>
-      <c r="H35" s="66"/>
-      <c r="I35" s="66"/>
-      <c r="J35" s="66"/>
-      <c r="K35" s="66"/>
-      <c r="L35" s="86"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="62"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="44"/>
+      <c r="L35" s="45"/>
       <c r="M35" s="1"/>
     </row>
     <row r="36" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="94" t="s">
+      <c r="C36" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="95"/>
-      <c r="E36" s="95"/>
-      <c r="F36" s="96"/>
-      <c r="G36" s="97" t="s">
+      <c r="D36" s="55"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="H36" s="98"/>
-      <c r="I36" s="98"/>
-      <c r="J36" s="98"/>
-      <c r="K36" s="98"/>
-      <c r="L36" s="99"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="58"/>
+      <c r="J36" s="58"/>
+      <c r="K36" s="58"/>
+      <c r="L36" s="59"/>
       <c r="M36" s="1"/>
     </row>
     <row r="37" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="85" t="s">
+      <c r="C37" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="66"/>
-      <c r="E37" s="66"/>
-      <c r="F37" s="86"/>
-      <c r="G37" s="85"/>
-      <c r="H37" s="66"/>
-      <c r="I37" s="66"/>
-      <c r="J37" s="66"/>
-      <c r="K37" s="66"/>
-      <c r="L37" s="86"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="44"/>
+      <c r="K37" s="44"/>
+      <c r="L37" s="45"/>
       <c r="M37" s="1"/>
     </row>
     <row r="38" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
-      <c r="B38" s="100" t="s">
+      <c r="B38" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="101"/>
-      <c r="D38" s="101"/>
-      <c r="E38" s="101"/>
-      <c r="F38" s="101"/>
-      <c r="G38" s="101"/>
-      <c r="H38" s="101"/>
-      <c r="I38" s="101"/>
-      <c r="J38" s="101"/>
-      <c r="K38" s="101"/>
-      <c r="L38" s="102"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="50"/>
+      <c r="K38" s="50"/>
+      <c r="L38" s="51"/>
       <c r="M38" s="1"/>
     </row>
     <row r="39" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D39" s="16" t="s">
+      <c r="D39" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E39" s="16" t="s">
+      <c r="E39" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F39" s="16" t="s">
+      <c r="F39" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G39" s="17" t="s">
+      <c r="G39" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="H39" s="17" t="s">
+      <c r="H39" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="I39" s="16" t="s">
+      <c r="I39" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="J39" s="25" t="s">
+      <c r="J39" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="K39" s="103" t="s">
+      <c r="K39" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="L39" s="104"/>
+      <c r="L39" s="53"/>
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C40" s="18" t="s">
+      <c r="C40" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="G40" s="105" t="s">
-        <v>49</v>
-      </c>
-      <c r="H40" s="105"/>
-      <c r="I40" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="J40" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="K40" s="85"/>
-      <c r="L40" s="86"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="120" t="s">
+        <v>97</v>
+      </c>
+      <c r="G40" t="s">
+        <v>101</v>
+      </c>
+      <c r="H40" s="121" t="s">
+        <v>96</v>
+      </c>
+      <c r="I40" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="J40" s="119" t="s">
+        <v>99</v>
+      </c>
+      <c r="K40" s="43"/>
+      <c r="L40" s="45"/>
       <c r="M40" s="1"/>
     </row>
     <row r="41" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="106"/>
-      <c r="H41" s="106"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="24" t="s">
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="124" t="s">
+        <v>95</v>
+      </c>
+      <c r="H41" s="122"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="K41" s="85"/>
-      <c r="L41" s="86"/>
+      <c r="K41" s="43"/>
+      <c r="L41" s="45"/>
       <c r="M41" s="1"/>
     </row>
     <row r="42" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="106"/>
-      <c r="H42" s="106"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="24"/>
-      <c r="K42" s="85"/>
-      <c r="L42" s="86"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="125" t="s">
+        <v>102</v>
+      </c>
+      <c r="H42" s="122"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="23"/>
+      <c r="K42" s="43"/>
+      <c r="L42" s="45"/>
       <c r="M42" s="1"/>
     </row>
     <row r="43" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="106"/>
-      <c r="H43" s="106"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="24"/>
-      <c r="K43" s="22"/>
-      <c r="L43" s="23"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="125"/>
+      <c r="H43" s="122"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="23"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="22"/>
       <c r="M43" s="1"/>
     </row>
     <row r="44" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="106"/>
-      <c r="H44" s="106"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="24"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="23"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="125"/>
+      <c r="H44" s="122"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="23"/>
+      <c r="K44" s="21"/>
+      <c r="L44" s="22"/>
       <c r="M44" s="1"/>
     </row>
     <row r="45" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="106"/>
-      <c r="H45" s="106"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="24"/>
-      <c r="K45" s="22"/>
-      <c r="L45" s="23"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="125"/>
+      <c r="H45" s="122"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="23"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="22"/>
       <c r="M45" s="1"/>
     </row>
     <row r="46" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="106"/>
-      <c r="H46" s="106"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="24"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="23"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="125"/>
+      <c r="H46" s="122"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="23"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="22"/>
       <c r="M46" s="1"/>
     </row>
     <row r="47" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="106"/>
-      <c r="H47" s="106"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="24"/>
-      <c r="K47" s="22"/>
-      <c r="L47" s="23"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="125"/>
+      <c r="H47" s="122"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="23"/>
+      <c r="K47" s="21"/>
+      <c r="L47" s="22"/>
       <c r="M47" s="1"/>
     </row>
     <row r="48" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="106"/>
-      <c r="H48" s="106"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="24"/>
-      <c r="K48" s="22"/>
-      <c r="L48" s="23"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="125"/>
+      <c r="H48" s="122"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="23"/>
+      <c r="K48" s="21"/>
+      <c r="L48" s="22"/>
       <c r="M48" s="1"/>
     </row>
     <row r="49" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A49" s="1"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="106"/>
-      <c r="H49" s="106"/>
-      <c r="I49" s="18"/>
-      <c r="J49" s="24"/>
-      <c r="K49" s="85"/>
-      <c r="L49" s="86"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="125"/>
+      <c r="H49" s="122"/>
+      <c r="I49" s="17"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="43"/>
+      <c r="L49" s="45"/>
       <c r="M49" s="1"/>
     </row>
     <row r="50" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A50" s="1"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="106"/>
-      <c r="H50" s="106"/>
-      <c r="I50" s="18"/>
-      <c r="J50" s="24"/>
-      <c r="K50" s="22"/>
-      <c r="L50" s="23"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="125"/>
+      <c r="H50" s="122"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="23"/>
+      <c r="K50" s="21"/>
+      <c r="L50" s="22"/>
       <c r="M50" s="1"/>
     </row>
     <row r="51" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="106"/>
-      <c r="H51" s="106"/>
-      <c r="I51" s="18"/>
-      <c r="J51" s="24"/>
-      <c r="K51" s="85"/>
-      <c r="L51" s="86"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="125"/>
+      <c r="H51" s="122"/>
+      <c r="I51" s="17"/>
+      <c r="J51" s="23"/>
+      <c r="K51" s="43"/>
+      <c r="L51" s="45"/>
       <c r="M51" s="1"/>
     </row>
     <row r="52" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A52" s="1"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="106"/>
-      <c r="H52" s="106"/>
-      <c r="I52" s="18"/>
-      <c r="J52" s="24"/>
-      <c r="K52" s="22"/>
-      <c r="L52" s="23"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="125"/>
+      <c r="H52" s="122"/>
+      <c r="I52" s="17"/>
+      <c r="J52" s="23"/>
+      <c r="K52" s="21"/>
+      <c r="L52" s="22"/>
       <c r="M52" s="1"/>
     </row>
     <row r="53" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A53" s="1"/>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="106"/>
-      <c r="H53" s="106"/>
-      <c r="I53" s="18"/>
-      <c r="J53" s="24"/>
-      <c r="K53" s="85"/>
-      <c r="L53" s="86"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="125"/>
+      <c r="H53" s="122"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="23"/>
+      <c r="K53" s="43"/>
+      <c r="L53" s="45"/>
       <c r="M53" s="1"/>
     </row>
     <row r="54" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A54" s="1"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="107"/>
-      <c r="H54" s="107"/>
-      <c r="I54" s="18"/>
-      <c r="J54" s="24"/>
-      <c r="K54" s="85"/>
-      <c r="L54" s="86"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="126"/>
+      <c r="H54" s="123"/>
+      <c r="I54" s="17"/>
+      <c r="J54" s="23"/>
+      <c r="K54" s="43"/>
+      <c r="L54" s="45"/>
       <c r="M54" s="1"/>
     </row>
     <row r="55" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1"/>
-      <c r="B55" s="19" t="s">
+      <c r="B55" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C55" s="108" t="s">
+      <c r="C55" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="D55" s="109"/>
-      <c r="E55" s="109"/>
-      <c r="F55" s="110"/>
-      <c r="G55" s="100" t="s">
+      <c r="D55" s="47"/>
+      <c r="E55" s="47"/>
+      <c r="F55" s="48"/>
+      <c r="G55" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="H55" s="101"/>
-      <c r="I55" s="101"/>
-      <c r="J55" s="101"/>
-      <c r="K55" s="101"/>
-      <c r="L55" s="102"/>
+      <c r="H55" s="50"/>
+      <c r="I55" s="50"/>
+      <c r="J55" s="50"/>
+      <c r="K55" s="50"/>
+      <c r="L55" s="51"/>
       <c r="M55" s="1"/>
     </row>
     <row r="56" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A56" s="1"/>
-      <c r="B56" s="20" t="s">
+      <c r="B56" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C56" s="85" t="s">
+      <c r="C56" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="D56" s="44"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="45"/>
+      <c r="G56" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="D56" s="66"/>
-      <c r="E56" s="66"/>
-      <c r="F56" s="86"/>
-      <c r="G56" s="85" t="s">
-        <v>91</v>
-      </c>
-      <c r="H56" s="66"/>
-      <c r="I56" s="66"/>
-      <c r="J56" s="66"/>
-      <c r="K56" s="66"/>
-      <c r="L56" s="86"/>
+      <c r="H56" s="44"/>
+      <c r="I56" s="44"/>
+      <c r="J56" s="44"/>
+      <c r="K56" s="44"/>
+      <c r="L56" s="45"/>
       <c r="M56" s="1"/>
     </row>
     <row r="57" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A57" s="1"/>
-      <c r="B57" s="21" t="s">
+      <c r="B57" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C57" s="111" t="s">
+      <c r="C57" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D57" s="35"/>
+      <c r="E57" s="35"/>
+      <c r="F57" s="36"/>
+      <c r="G57" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="D57" s="112"/>
-      <c r="E57" s="112"/>
-      <c r="F57" s="113"/>
-      <c r="G57" s="111" t="s">
-        <v>93</v>
-      </c>
-      <c r="H57" s="112"/>
-      <c r="I57" s="112"/>
-      <c r="J57" s="112"/>
-      <c r="K57" s="112"/>
-      <c r="L57" s="113"/>
+      <c r="H57" s="35"/>
+      <c r="I57" s="35"/>
+      <c r="J57" s="35"/>
+      <c r="K57" s="35"/>
+      <c r="L57" s="36"/>
       <c r="M57" s="1"/>
     </row>
     <row r="58" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A58" s="1"/>
-      <c r="B58" s="21" t="s">
+      <c r="B58" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C58" s="111" t="s">
+      <c r="C58" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D58" s="35"/>
+      <c r="E58" s="35"/>
+      <c r="F58" s="36"/>
+      <c r="G58" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="D58" s="112"/>
-      <c r="E58" s="112"/>
-      <c r="F58" s="113"/>
-      <c r="G58" s="111" t="s">
-        <v>95</v>
-      </c>
-      <c r="H58" s="112"/>
-      <c r="I58" s="112"/>
-      <c r="J58" s="112"/>
-      <c r="K58" s="112"/>
-      <c r="L58" s="113"/>
+      <c r="H58" s="35"/>
+      <c r="I58" s="35"/>
+      <c r="J58" s="35"/>
+      <c r="K58" s="35"/>
+      <c r="L58" s="36"/>
       <c r="M58" s="1"/>
     </row>
     <row r="59" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A59" s="1"/>
-      <c r="B59" s="114" t="s">
+      <c r="B59" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C59" s="115"/>
-      <c r="D59" s="115"/>
-      <c r="E59" s="115"/>
-      <c r="F59" s="115"/>
-      <c r="G59" s="115"/>
-      <c r="H59" s="115"/>
-      <c r="I59" s="115"/>
-      <c r="J59" s="115"/>
-      <c r="K59" s="115"/>
-      <c r="L59" s="116"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="26"/>
+      <c r="G59" s="26"/>
+      <c r="H59" s="26"/>
+      <c r="I59" s="26"/>
+      <c r="J59" s="26"/>
+      <c r="K59" s="26"/>
+      <c r="L59" s="27"/>
       <c r="M59" s="1"/>
     </row>
     <row r="60" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1"/>
-      <c r="B60" s="87" t="s">
+      <c r="B60" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="C60" s="88"/>
-      <c r="D60" s="88"/>
-      <c r="E60" s="88"/>
-      <c r="F60" s="89"/>
-      <c r="G60" s="90" t="s">
+      <c r="C60" s="38"/>
+      <c r="D60" s="38"/>
+      <c r="E60" s="38"/>
+      <c r="F60" s="39"/>
+      <c r="G60" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="H60" s="91"/>
-      <c r="I60" s="91"/>
-      <c r="J60" s="91"/>
-      <c r="K60" s="91"/>
-      <c r="L60" s="92"/>
+      <c r="H60" s="41"/>
+      <c r="I60" s="41"/>
+      <c r="J60" s="41"/>
+      <c r="K60" s="41"/>
+      <c r="L60" s="42"/>
       <c r="M60" s="1"/>
     </row>
     <row r="61" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A61" s="1"/>
-      <c r="B61" s="85"/>
-      <c r="C61" s="66"/>
-      <c r="D61" s="66"/>
-      <c r="E61" s="66"/>
-      <c r="F61" s="86"/>
-      <c r="G61" s="85"/>
-      <c r="H61" s="66"/>
-      <c r="I61" s="66"/>
-      <c r="J61" s="66"/>
-      <c r="K61" s="66"/>
-      <c r="L61" s="86"/>
+      <c r="B61" s="43"/>
+      <c r="C61" s="44"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="44"/>
+      <c r="F61" s="45"/>
+      <c r="G61" s="43"/>
+      <c r="H61" s="44"/>
+      <c r="I61" s="44"/>
+      <c r="J61" s="44"/>
+      <c r="K61" s="44"/>
+      <c r="L61" s="45"/>
       <c r="M61" s="1"/>
     </row>
     <row r="62" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A62" s="1"/>
-      <c r="B62" s="114" t="s">
+      <c r="B62" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C62" s="115"/>
-      <c r="D62" s="115"/>
-      <c r="E62" s="115"/>
-      <c r="F62" s="115"/>
-      <c r="G62" s="115"/>
-      <c r="H62" s="115"/>
-      <c r="I62" s="115"/>
-      <c r="J62" s="115"/>
-      <c r="K62" s="115"/>
-      <c r="L62" s="116"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="26"/>
+      <c r="I62" s="26"/>
+      <c r="J62" s="26"/>
+      <c r="K62" s="26"/>
+      <c r="L62" s="27"/>
       <c r="M62" s="1"/>
     </row>
     <row r="63" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A63" s="1"/>
-      <c r="B63" s="117"/>
-      <c r="C63" s="118"/>
-      <c r="D63" s="118"/>
-      <c r="E63" s="118"/>
-      <c r="F63" s="118"/>
-      <c r="G63" s="118"/>
-      <c r="H63" s="118"/>
-      <c r="I63" s="118"/>
-      <c r="J63" s="118"/>
-      <c r="K63" s="118"/>
-      <c r="L63" s="119"/>
+      <c r="B63" s="28"/>
+      <c r="C63" s="29"/>
+      <c r="D63" s="29"/>
+      <c r="E63" s="29"/>
+      <c r="F63" s="29"/>
+      <c r="G63" s="29"/>
+      <c r="H63" s="29"/>
+      <c r="I63" s="29"/>
+      <c r="J63" s="29"/>
+      <c r="K63" s="29"/>
+      <c r="L63" s="30"/>
       <c r="M63" s="1"/>
     </row>
     <row r="64" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A64" s="1"/>
-      <c r="B64" s="120"/>
-      <c r="C64" s="121"/>
-      <c r="D64" s="121"/>
-      <c r="E64" s="121"/>
-      <c r="F64" s="121"/>
-      <c r="G64" s="121"/>
-      <c r="H64" s="121"/>
-      <c r="I64" s="121"/>
-      <c r="J64" s="121"/>
-      <c r="K64" s="121"/>
-      <c r="L64" s="122"/>
+      <c r="B64" s="31"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="32"/>
+      <c r="G64" s="32"/>
+      <c r="H64" s="32"/>
+      <c r="I64" s="32"/>
+      <c r="J64" s="32"/>
+      <c r="K64" s="32"/>
+      <c r="L64" s="33"/>
       <c r="M64" s="1"/>
     </row>
     <row r="65" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
@@ -2925,7 +3206,85 @@
     <row r="85" ht="14.5" x14ac:dyDescent="0.35"/>
     <row r="86" ht="14.5" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="88">
+  <mergeCells count="87">
+    <mergeCell ref="H40:H54"/>
+    <mergeCell ref="B2:F5"/>
+    <mergeCell ref="G2:L5"/>
+    <mergeCell ref="B6:L6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="H9:L9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="G10:L10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="G14:L16"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="G17:L17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="G18:L18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="G19:L19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="G20:L20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="G21:L21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="G22:L22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="G23:L23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="G24:L24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="G25:L25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="G26:L26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="G27:L27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="G28:L28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="G29:L29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="G30:L30"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="G32:L32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="G33:L33"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="G34:L34"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="G35:L35"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="G36:L36"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="G37:L37"/>
+    <mergeCell ref="B38:L38"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="C55:F55"/>
+    <mergeCell ref="G55:L55"/>
+    <mergeCell ref="C56:F56"/>
+    <mergeCell ref="G56:L56"/>
+    <mergeCell ref="C57:F57"/>
+    <mergeCell ref="G57:L57"/>
     <mergeCell ref="B62:L62"/>
     <mergeCell ref="B63:L64"/>
     <mergeCell ref="C58:F58"/>
@@ -2935,87 +3294,8 @@
     <mergeCell ref="G60:L60"/>
     <mergeCell ref="B61:F61"/>
     <mergeCell ref="G61:L61"/>
-    <mergeCell ref="C55:F55"/>
-    <mergeCell ref="G55:L55"/>
-    <mergeCell ref="C56:F56"/>
-    <mergeCell ref="G56:L56"/>
-    <mergeCell ref="C57:F57"/>
-    <mergeCell ref="G57:L57"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="G40:G54"/>
-    <mergeCell ref="H40:H54"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="K41:L41"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="G36:L36"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="G37:L37"/>
-    <mergeCell ref="B38:L38"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="G33:L33"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="G34:L34"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="G35:L35"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="G30:L30"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="G32:L32"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="G27:L27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="G28:L28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="G29:L29"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="G24:L24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="G25:L25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="G26:L26"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="G21:L21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="G22:L22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="G23:L23"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="G18:L18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="G19:L19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="G20:L20"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="G14:L16"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="G17:L17"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="H9:L9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="G10:L10"/>
-    <mergeCell ref="B2:F5"/>
-    <mergeCell ref="G2:L5"/>
-    <mergeCell ref="B6:L6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="H7:L7"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="C8:L8">
     <cfRule type="expression" priority="30" stopIfTrue="1">
       <formula>LEN($C$8)=0</formula>
@@ -3064,14 +3344,6 @@
       <formula>LEN($G$25)&gt;32</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F40">
-    <cfRule type="expression" dxfId="9" priority="19" stopIfTrue="1">
-      <formula>LEN($B$40)&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" priority="20" stopIfTrue="1">
-      <formula>LEN($F$40)&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F41:F43 F50:F54 F46:F47">
     <cfRule type="expression" priority="17" stopIfTrue="1">
       <formula>LEN(F41)&gt;0</formula>
@@ -3086,22 +3358,6 @@
     </cfRule>
     <cfRule type="expression" dxfId="7" priority="16" stopIfTrue="1">
       <formula>LEN($C$8)&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G40">
-    <cfRule type="expression" dxfId="6" priority="13" stopIfTrue="1">
-      <formula>LEN($B$40)&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" priority="14" stopIfTrue="1">
-      <formula>LEN($F$40)&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I40:J40">
-    <cfRule type="expression" dxfId="5" priority="11" stopIfTrue="1">
-      <formula>LEN($B$40)&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" priority="12" stopIfTrue="1">
-      <formula>LEN($F$40)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:F11">
@@ -3166,15 +3422,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100523544B2F623FE47B58BA7FA2901C425" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="85d2b0da6cf4d3f4433d3933320c8674">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b7c6738d-b7b8-47ce-b62e-d9222222e52e" xmlns:ns4="8259444a-4876-4f9e-a4da-1fddcbb819b8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c4d24f5b67c1beeba694d271a03c59b0" ns3:_="" ns4:_="">
     <xsd:import namespace="b7c6738d-b7b8-47ce-b62e-d9222222e52e"/>
@@ -3351,6 +3598,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3358,14 +3614,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33C41FCB-279C-450E-81D1-E323F4CA622F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74471590-99F1-4F51-98CD-812CDDD957B5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3384,6 +3632,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33C41FCB-279C-450E-81D1-E323F4CA622F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3942C816-0066-4A4E-9CBE-620D36D4718B}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
God download draft BL working
</commit_message>
<xml_diff>
--- a/AmbRcnTradeServer/ExcelTemplates/Maersk Draft BL Template BL.xlsx
+++ b/AmbRcnTradeServer/ExcelTemplates/Maersk Draft BL Template BL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Visual Studio\AmbRcnTrade\AmbRcnTradeServer\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6961EFDF-C8AD-4A5C-87DE-0E722F247783}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFD106D-EC6C-4DF3-86F4-C33D23029927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="10680" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
   <si>
     <t>Shipping Instruction submitter (who should Safmarine Line contact in case of  any queries to this document)</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>Particulars as furnished by shipper – Carrier not responsible (Please insert Rows for more information)</t>
-  </si>
-  <si>
-    <t>Container number*</t>
   </si>
   <si>
     <t>Carrier Seal*</t>
@@ -336,6 +333,9 @@
   </si>
   <si>
     <t>BillLading.PreCargoDescription.Footer</t>
+  </si>
+  <si>
+    <t>Container.Rows</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -860,11 +860,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -908,20 +917,17 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1125,22 +1131,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -1234,38 +1224,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -1273,7 +1273,98 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="51">
+  <dxfs count="64">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1967,8 +2058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -2004,79 +2095,79 @@
     </row>
     <row r="2" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="95"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="106"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="101"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
-      <c r="J3" s="108"/>
-      <c r="K3" s="108"/>
-      <c r="L3" s="109"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="103"/>
+      <c r="J3" s="103"/>
+      <c r="K3" s="103"/>
+      <c r="L3" s="104"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
-      <c r="B4" s="98"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="107"/>
-      <c r="H4" s="108"/>
-      <c r="I4" s="108"/>
-      <c r="J4" s="108"/>
-      <c r="K4" s="108"/>
-      <c r="L4" s="109"/>
+      <c r="B4" s="93"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="95"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="103"/>
+      <c r="K4" s="103"/>
+      <c r="L4" s="104"/>
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1"/>
-      <c r="B5" s="101"/>
-      <c r="C5" s="102"/>
-      <c r="D5" s="102"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="103"/>
-      <c r="G5" s="110"/>
-      <c r="H5" s="111"/>
-      <c r="I5" s="111"/>
-      <c r="J5" s="111"/>
-      <c r="K5" s="111"/>
-      <c r="L5" s="112"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="105"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="106"/>
+      <c r="J5" s="106"/>
+      <c r="K5" s="106"/>
+      <c r="L5" s="107"/>
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1"/>
-      <c r="B6" s="113" t="s">
+      <c r="B6" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="114"/>
-      <c r="D6" s="114"/>
-      <c r="E6" s="114"/>
-      <c r="F6" s="114"/>
-      <c r="G6" s="114"/>
-      <c r="H6" s="114"/>
-      <c r="I6" s="114"/>
-      <c r="J6" s="114"/>
-      <c r="K6" s="114"/>
-      <c r="L6" s="115"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="110"/>
       <c r="M6" s="1"/>
       <c r="N6" s="2"/>
     </row>
@@ -2085,20 +2176,20 @@
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="89" t="s">
+      <c r="C7" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="91"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="86"/>
       <c r="G7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="116"/>
-      <c r="I7" s="117"/>
-      <c r="J7" s="117"/>
-      <c r="K7" s="117"/>
-      <c r="L7" s="118"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="112"/>
+      <c r="J7" s="112"/>
+      <c r="K7" s="112"/>
+      <c r="L7" s="113"/>
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2106,18 +2197,18 @@
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="89" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="90"/>
-      <c r="E8" s="90"/>
-      <c r="F8" s="90"/>
-      <c r="G8" s="90"/>
-      <c r="H8" s="90"/>
-      <c r="I8" s="90"/>
-      <c r="J8" s="90"/>
-      <c r="K8" s="90"/>
-      <c r="L8" s="91"/>
+      <c r="C8" s="84" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="85"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="85"/>
+      <c r="I8" s="85"/>
+      <c r="J8" s="85"/>
+      <c r="K8" s="85"/>
+      <c r="L8" s="86"/>
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2125,424 +2216,424 @@
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="89" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="91"/>
+      <c r="C9" s="84" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="85"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="86"/>
       <c r="G9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="89">
+      <c r="H9" s="84">
         <v>3</v>
       </c>
-      <c r="I9" s="90"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="91"/>
+      <c r="I9" s="85"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="85"/>
+      <c r="L9" s="86"/>
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="1"/>
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="92" t="s">
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="93"/>
-      <c r="I10" s="93"/>
-      <c r="J10" s="93"/>
-      <c r="K10" s="93"/>
-      <c r="L10" s="94"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="88"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="88"/>
+      <c r="L10" s="89"/>
       <c r="M10" s="6"/>
       <c r="N10" s="7"/>
     </row>
     <row r="11" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
-      <c r="B11" s="68" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
+      <c r="B11" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="69"/>
       <c r="G11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="85" t="s">
-        <v>56</v>
-      </c>
-      <c r="I11" s="86"/>
-      <c r="J11" s="86"/>
-      <c r="K11" s="86"/>
-      <c r="L11" s="87"/>
+      <c r="H11" s="123" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="124"/>
+      <c r="J11" s="124"/>
+      <c r="K11" s="124"/>
+      <c r="L11" s="125"/>
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
-      <c r="B12" s="63" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="64"/>
+      <c r="B12" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="63"/>
       <c r="G12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="60" t="s">
-        <v>57</v>
-      </c>
-      <c r="I12" s="61"/>
-      <c r="J12" s="61"/>
-      <c r="K12" s="61"/>
-      <c r="L12" s="88"/>
+      <c r="H12" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="63"/>
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
-      <c r="B13" s="63" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="64"/>
+      <c r="B13" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="63"/>
       <c r="G13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="I13" s="61"/>
-      <c r="J13" s="61"/>
-      <c r="K13" s="61"/>
-      <c r="L13" s="88"/>
+      <c r="H13" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="63"/>
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
-      <c r="B14" s="63" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="74" t="s">
+      <c r="B14" s="62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="75"/>
-      <c r="I14" s="75"/>
-      <c r="J14" s="75"/>
-      <c r="K14" s="75"/>
-      <c r="L14" s="76"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="74"/>
+      <c r="J14" s="74"/>
+      <c r="K14" s="74"/>
+      <c r="L14" s="75"/>
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
-      <c r="B15" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="77"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="78"/>
-      <c r="J15" s="78"/>
-      <c r="K15" s="78"/>
-      <c r="L15" s="79"/>
+      <c r="B15" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="77"/>
+      <c r="I15" s="77"/>
+      <c r="J15" s="77"/>
+      <c r="K15" s="77"/>
+      <c r="L15" s="78"/>
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="1"/>
-      <c r="B16" s="63" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="80"/>
-      <c r="H16" s="81"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="81"/>
-      <c r="L16" s="82"/>
+      <c r="B16" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="80"/>
+      <c r="I16" s="80"/>
+      <c r="J16" s="80"/>
+      <c r="K16" s="80"/>
+      <c r="L16" s="81"/>
       <c r="M16" s="1"/>
     </row>
     <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1"/>
-      <c r="B17" s="83" t="s">
+      <c r="B17" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="84"/>
-      <c r="G17" s="83" t="s">
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="66"/>
-      <c r="I17" s="66"/>
-      <c r="J17" s="66"/>
-      <c r="K17" s="66"/>
-      <c r="L17" s="84"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="65"/>
+      <c r="L17" s="83"/>
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
-      <c r="B18" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="69"/>
-      <c r="D18" s="69"/>
-      <c r="E18" s="69"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="68" t="s">
-        <v>83</v>
-      </c>
-      <c r="H18" s="69"/>
-      <c r="I18" s="69"/>
-      <c r="J18" s="69"/>
-      <c r="K18" s="69"/>
-      <c r="L18" s="70"/>
+      <c r="B18" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="68"/>
+      <c r="L18" s="69"/>
       <c r="M18" s="1"/>
     </row>
     <row r="19" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
-      <c r="B19" s="71" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="72"/>
-      <c r="D19" s="72"/>
-      <c r="E19" s="72"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="63" t="s">
-        <v>58</v>
-      </c>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="64"/>
+      <c r="B19" s="70" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="71"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="63"/>
       <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
-      <c r="B20" s="71" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="72"/>
-      <c r="D20" s="72"/>
-      <c r="E20" s="72"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="63" t="s">
-        <v>59</v>
-      </c>
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
-      <c r="K20" s="44"/>
-      <c r="L20" s="64"/>
+      <c r="B20" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="63"/>
       <c r="M20" s="1"/>
     </row>
     <row r="21" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
-      <c r="B21" s="71" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="73"/>
-      <c r="G21" s="63" t="s">
-        <v>60</v>
-      </c>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="64"/>
+      <c r="B21" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="63"/>
       <c r="M21" s="1"/>
     </row>
     <row r="22" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
-      <c r="B22" s="71" t="s">
-        <v>73</v>
-      </c>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="63" t="s">
-        <v>61</v>
-      </c>
-      <c r="H22" s="44"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="44"/>
-      <c r="K22" s="44"/>
-      <c r="L22" s="64"/>
+      <c r="B22" s="70" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="71"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="62" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="63"/>
       <c r="M22" s="1"/>
     </row>
     <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="1"/>
-      <c r="B23" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="44"/>
-      <c r="L23" s="64"/>
+      <c r="B23" s="70" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="71"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="63"/>
       <c r="M23" s="1"/>
     </row>
     <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="1"/>
-      <c r="B24" s="65" t="s">
+      <c r="B24" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="66"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="65" t="s">
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="H24" s="66"/>
-      <c r="I24" s="66"/>
-      <c r="J24" s="66"/>
-      <c r="K24" s="66"/>
-      <c r="L24" s="67"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="65"/>
+      <c r="L24" s="66"/>
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
-      <c r="B25" s="68" t="s">
+      <c r="B25" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="68"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="69"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="70"/>
-      <c r="G25" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="H25" s="69"/>
-      <c r="I25" s="69"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="69"/>
-      <c r="L25" s="70"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="68"/>
+      <c r="L25" s="69"/>
       <c r="M25" s="1"/>
     </row>
     <row r="26" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
-      <c r="B26" s="63" t="s">
-        <v>84</v>
-      </c>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="64"/>
-      <c r="G26" s="63" t="s">
-        <v>77</v>
-      </c>
-      <c r="H26" s="44"/>
-      <c r="I26" s="44"/>
-      <c r="J26" s="44"/>
-      <c r="K26" s="44"/>
-      <c r="L26" s="64"/>
+      <c r="B26" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="63"/>
       <c r="M26" s="1"/>
     </row>
     <row r="27" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
-      <c r="B27" s="63" t="s">
-        <v>85</v>
-      </c>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="63" t="s">
-        <v>78</v>
-      </c>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="44"/>
-      <c r="L27" s="64"/>
+      <c r="B27" s="62" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="63"/>
       <c r="M27" s="1"/>
     </row>
     <row r="28" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
-      <c r="B28" s="63" t="s">
-        <v>86</v>
-      </c>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="63" t="s">
-        <v>79</v>
-      </c>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="44"/>
-      <c r="K28" s="44"/>
-      <c r="L28" s="64"/>
+      <c r="B28" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="63"/>
+      <c r="G28" s="62" t="s">
+        <v>78</v>
+      </c>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="43"/>
+      <c r="L28" s="63"/>
       <c r="M28" s="1"/>
     </row>
     <row r="29" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
-      <c r="B29" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="64"/>
-      <c r="G29" s="63" t="s">
-        <v>80</v>
-      </c>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="64"/>
+      <c r="B29" s="62" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="43"/>
+      <c r="L29" s="63"/>
       <c r="M29" s="1"/>
     </row>
     <row r="30" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
-      <c r="B30" s="63" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="63" t="s">
-        <v>81</v>
-      </c>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
-      <c r="K30" s="44"/>
-      <c r="L30" s="64"/>
+      <c r="B30" s="62" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="43"/>
+      <c r="L30" s="63"/>
       <c r="M30" s="1"/>
     </row>
     <row r="31" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
@@ -2550,58 +2641,58 @@
       <c r="B31" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" s="44"/>
-      <c r="E31" s="44"/>
-      <c r="F31" s="45"/>
+      <c r="C31" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="44"/>
       <c r="G31" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H31" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="I31" s="44"/>
-      <c r="J31" s="44"/>
-      <c r="K31" s="44"/>
-      <c r="L31" s="45"/>
+      <c r="H31" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="I31" s="43"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="43"/>
+      <c r="L31" s="44"/>
       <c r="M31" s="1"/>
     </row>
     <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="40" t="s">
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
-      <c r="J32" s="41"/>
-      <c r="K32" s="41"/>
-      <c r="L32" s="42"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="41"/>
       <c r="M32" s="1"/>
     </row>
     <row r="33" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
-      <c r="B33" s="60"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="62"/>
-      <c r="G33" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="H33" s="61"/>
-      <c r="I33" s="61"/>
-      <c r="J33" s="61"/>
-      <c r="K33" s="61"/>
-      <c r="L33" s="62"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="59" t="s">
+        <v>48</v>
+      </c>
+      <c r="H33" s="60"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="60"/>
+      <c r="K33" s="60"/>
+      <c r="L33" s="61"/>
       <c r="M33" s="1"/>
     </row>
     <row r="34" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2609,39 +2700,39 @@
       <c r="B34" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="54" t="s">
+      <c r="C34" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="55"/>
-      <c r="E34" s="55"/>
-      <c r="F34" s="56"/>
-      <c r="G34" s="57" t="s">
+      <c r="D34" s="54"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="58"/>
-      <c r="K34" s="58"/>
-      <c r="L34" s="59"/>
+      <c r="H34" s="57"/>
+      <c r="I34" s="57"/>
+      <c r="J34" s="57"/>
+      <c r="K34" s="57"/>
+      <c r="L34" s="58"/>
       <c r="M34" s="1"/>
     </row>
     <row r="35" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
-      <c r="B35" s="127" t="s">
-        <v>82</v>
-      </c>
-      <c r="C35" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35" s="61"/>
-      <c r="E35" s="61"/>
-      <c r="F35" s="62"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="44"/>
-      <c r="J35" s="44"/>
-      <c r="K35" s="44"/>
-      <c r="L35" s="45"/>
+      <c r="B35" s="114" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="60"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="42"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="43"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="44"/>
       <c r="M35" s="1"/>
     </row>
     <row r="36" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2649,565 +2740,401 @@
       <c r="B36" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="54" t="s">
+      <c r="C36" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="55"/>
-      <c r="E36" s="55"/>
-      <c r="F36" s="56"/>
-      <c r="G36" s="57" t="s">
+      <c r="D36" s="54"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="55"/>
+      <c r="G36" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="H36" s="58"/>
-      <c r="I36" s="58"/>
-      <c r="J36" s="58"/>
-      <c r="K36" s="58"/>
-      <c r="L36" s="59"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="57"/>
+      <c r="J36" s="57"/>
+      <c r="K36" s="57"/>
+      <c r="L36" s="58"/>
       <c r="M36" s="1"/>
     </row>
     <row r="37" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="44"/>
-      <c r="I37" s="44"/>
-      <c r="J37" s="44"/>
-      <c r="K37" s="44"/>
-      <c r="L37" s="45"/>
+        <v>47</v>
+      </c>
+      <c r="C37" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="43"/>
+      <c r="K37" s="43"/>
+      <c r="L37" s="44"/>
       <c r="M37" s="1"/>
     </row>
     <row r="38" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
-      <c r="B38" s="49" t="s">
+      <c r="B38" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="50"/>
-      <c r="D38" s="50"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="50"/>
-      <c r="G38" s="50"/>
-      <c r="H38" s="50"/>
-      <c r="I38" s="50"/>
-      <c r="J38" s="50"/>
-      <c r="K38" s="50"/>
-      <c r="L38" s="51"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="49"/>
+      <c r="L38" s="50"/>
       <c r="M38" s="1"/>
     </row>
     <row r="39" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="115"/>
+      <c r="C39" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="D39" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="E39" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E39" s="15" t="s">
+      <c r="F39" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F39" s="15" t="s">
+      <c r="G39" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G39" s="16" t="s">
+      <c r="H39" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="H39" s="16" t="s">
+      <c r="I39" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="I39" s="15" t="s">
+      <c r="J39" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="K39" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="J39" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="K39" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="L39" s="53"/>
+      <c r="L39" s="52"/>
       <c r="M39" s="1"/>
     </row>
     <row r="40" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="B40" s="17" t="s">
-        <v>49</v>
+        <v>102</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D40" s="17"/>
       <c r="E40" s="17"/>
-      <c r="F40" s="120" t="s">
+      <c r="K40" s="42"/>
+      <c r="L40" s="44"/>
+      <c r="M40" s="1"/>
+    </row>
+    <row r="41" spans="1:13" ht="67" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="1"/>
+      <c r="B41" s="116"/>
+      <c r="C41" s="116"/>
+      <c r="D41" s="116"/>
+      <c r="E41" s="116"/>
+      <c r="F41" s="119" t="s">
+        <v>96</v>
+      </c>
+      <c r="G41" s="114" t="s">
+        <v>100</v>
+      </c>
+      <c r="H41" s="120" t="s">
+        <v>95</v>
+      </c>
+      <c r="I41" s="116" t="s">
         <v>97</v>
       </c>
-      <c r="G40" t="s">
-        <v>101</v>
-      </c>
-      <c r="H40" s="121" t="s">
-        <v>96</v>
-      </c>
-      <c r="I40" s="17" t="s">
+      <c r="J41" s="117" t="s">
         <v>98</v>
       </c>
-      <c r="J40" s="119" t="s">
-        <v>99</v>
-      </c>
-      <c r="K40" s="43"/>
-      <c r="L40" s="45"/>
-      <c r="M40" s="1"/>
-    </row>
-    <row r="41" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="1"/>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="124" t="s">
-        <v>95</v>
-      </c>
-      <c r="H41" s="122"/>
-      <c r="I41" s="17"/>
-      <c r="J41" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="K41" s="43"/>
-      <c r="L41" s="45"/>
+      <c r="K41" s="42"/>
+      <c r="L41" s="44"/>
       <c r="M41" s="1"/>
     </row>
     <row r="42" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="125" t="s">
-        <v>102</v>
-      </c>
-      <c r="H42" s="122"/>
-      <c r="I42" s="17"/>
-      <c r="J42" s="23"/>
-      <c r="K42" s="43"/>
-      <c r="L42" s="45"/>
+      <c r="B42" s="116"/>
+      <c r="C42" s="116"/>
+      <c r="D42" s="116"/>
+      <c r="E42" s="116"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="118" t="s">
+        <v>94</v>
+      </c>
+      <c r="H42" s="121"/>
+      <c r="I42" s="116"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="42"/>
+      <c r="L42" s="44"/>
       <c r="M42" s="1"/>
     </row>
     <row r="43" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="125"/>
-      <c r="H43" s="122"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="23"/>
-      <c r="K43" s="21"/>
-      <c r="L43" s="22"/>
+      <c r="B43" s="116"/>
+      <c r="C43" s="116"/>
+      <c r="D43" s="116"/>
+      <c r="E43" s="116"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="122" t="s">
+        <v>101</v>
+      </c>
+      <c r="H43" s="121"/>
+      <c r="I43" s="116"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="22"/>
+      <c r="L43" s="23"/>
       <c r="M43" s="1"/>
     </row>
-    <row r="44" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="125"/>
-      <c r="H44" s="122"/>
-      <c r="I44" s="17"/>
-      <c r="J44" s="23"/>
-      <c r="K44" s="21"/>
-      <c r="L44" s="22"/>
+      <c r="B44" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" s="46"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="H44" s="49"/>
+      <c r="I44" s="49"/>
+      <c r="J44" s="49"/>
+      <c r="K44" s="49"/>
+      <c r="L44" s="50"/>
       <c r="M44" s="1"/>
     </row>
     <row r="45" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="125"/>
-      <c r="H45" s="122"/>
-      <c r="I45" s="17"/>
-      <c r="J45" s="23"/>
-      <c r="K45" s="21"/>
-      <c r="L45" s="22"/>
+      <c r="B45" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" s="43"/>
+      <c r="E45" s="43"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="H45" s="43"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
+      <c r="K45" s="43"/>
+      <c r="L45" s="44"/>
       <c r="M45" s="1"/>
     </row>
     <row r="46" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="125"/>
-      <c r="H46" s="122"/>
-      <c r="I46" s="17"/>
-      <c r="J46" s="23"/>
-      <c r="K46" s="21"/>
-      <c r="L46" s="22"/>
+      <c r="B46" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="D46" s="34"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="H46" s="34"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
+      <c r="K46" s="34"/>
+      <c r="L46" s="35"/>
       <c r="M46" s="1"/>
     </row>
     <row r="47" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="125"/>
-      <c r="H47" s="122"/>
-      <c r="I47" s="17"/>
-      <c r="J47" s="23"/>
-      <c r="K47" s="21"/>
-      <c r="L47" s="22"/>
+      <c r="B47" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D47" s="34"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="H47" s="34"/>
+      <c r="I47" s="34"/>
+      <c r="J47" s="34"/>
+      <c r="K47" s="34"/>
+      <c r="L47" s="35"/>
       <c r="M47" s="1"/>
     </row>
     <row r="48" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="125"/>
-      <c r="H48" s="122"/>
-      <c r="I48" s="17"/>
-      <c r="J48" s="23"/>
-      <c r="K48" s="21"/>
-      <c r="L48" s="22"/>
+      <c r="B48" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" s="25"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="25"/>
+      <c r="I48" s="25"/>
+      <c r="J48" s="25"/>
+      <c r="K48" s="25"/>
+      <c r="L48" s="26"/>
       <c r="M48" s="1"/>
     </row>
-    <row r="49" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="125"/>
-      <c r="H49" s="122"/>
-      <c r="I49" s="17"/>
-      <c r="J49" s="23"/>
-      <c r="K49" s="43"/>
-      <c r="L49" s="45"/>
+      <c r="B49" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="38"/>
+      <c r="G49" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="H49" s="40"/>
+      <c r="I49" s="40"/>
+      <c r="J49" s="40"/>
+      <c r="K49" s="40"/>
+      <c r="L49" s="41"/>
       <c r="M49" s="1"/>
     </row>
     <row r="50" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A50" s="1"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="125"/>
-      <c r="H50" s="122"/>
-      <c r="I50" s="17"/>
-      <c r="J50" s="23"/>
-      <c r="K50" s="21"/>
-      <c r="L50" s="22"/>
+      <c r="B50" s="42"/>
+      <c r="C50" s="43"/>
+      <c r="D50" s="43"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="42"/>
+      <c r="H50" s="43"/>
+      <c r="I50" s="43"/>
+      <c r="J50" s="43"/>
+      <c r="K50" s="43"/>
+      <c r="L50" s="44"/>
       <c r="M50" s="1"/>
     </row>
     <row r="51" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="125"/>
-      <c r="H51" s="122"/>
-      <c r="I51" s="17"/>
-      <c r="J51" s="23"/>
-      <c r="K51" s="43"/>
-      <c r="L51" s="45"/>
+      <c r="B51" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" s="25"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="25"/>
+      <c r="J51" s="25"/>
+      <c r="K51" s="25"/>
+      <c r="L51" s="26"/>
       <c r="M51" s="1"/>
     </row>
     <row r="52" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A52" s="1"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="17"/>
-      <c r="G52" s="125"/>
-      <c r="H52" s="122"/>
-      <c r="I52" s="17"/>
-      <c r="J52" s="23"/>
-      <c r="K52" s="21"/>
-      <c r="L52" s="22"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="28"/>
+      <c r="H52" s="28"/>
+      <c r="I52" s="28"/>
+      <c r="J52" s="28"/>
+      <c r="K52" s="28"/>
+      <c r="L52" s="29"/>
       <c r="M52" s="1"/>
     </row>
     <row r="53" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A53" s="1"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17"/>
-      <c r="G53" s="125"/>
-      <c r="H53" s="122"/>
-      <c r="I53" s="17"/>
-      <c r="J53" s="23"/>
-      <c r="K53" s="43"/>
-      <c r="L53" s="45"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="31"/>
+      <c r="G53" s="31"/>
+      <c r="H53" s="31"/>
+      <c r="I53" s="31"/>
+      <c r="J53" s="31"/>
+      <c r="K53" s="31"/>
+      <c r="L53" s="32"/>
       <c r="M53" s="1"/>
     </row>
     <row r="54" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A54" s="1"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="17"/>
-      <c r="G54" s="126"/>
-      <c r="H54" s="123"/>
-      <c r="I54" s="17"/>
-      <c r="J54" s="23"/>
-      <c r="K54" s="43"/>
-      <c r="L54" s="45"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
       <c r="M54" s="1"/>
     </row>
-    <row r="55" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A55" s="1"/>
-      <c r="B55" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C55" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="D55" s="47"/>
-      <c r="E55" s="47"/>
-      <c r="F55" s="48"/>
-      <c r="G55" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="H55" s="50"/>
-      <c r="I55" s="50"/>
-      <c r="J55" s="50"/>
-      <c r="K55" s="50"/>
-      <c r="L55" s="51"/>
       <c r="M55" s="1"/>
     </row>
     <row r="56" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A56" s="1"/>
-      <c r="B56" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C56" s="43" t="s">
-        <v>89</v>
-      </c>
-      <c r="D56" s="44"/>
-      <c r="E56" s="44"/>
-      <c r="F56" s="45"/>
-      <c r="G56" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="H56" s="44"/>
-      <c r="I56" s="44"/>
-      <c r="J56" s="44"/>
-      <c r="K56" s="44"/>
-      <c r="L56" s="45"/>
       <c r="M56" s="1"/>
     </row>
-    <row r="57" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="1"/>
-      <c r="B57" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C57" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="D57" s="35"/>
-      <c r="E57" s="35"/>
-      <c r="F57" s="36"/>
-      <c r="G57" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="H57" s="35"/>
-      <c r="I57" s="35"/>
-      <c r="J57" s="35"/>
-      <c r="K57" s="35"/>
-      <c r="L57" s="36"/>
-      <c r="M57" s="1"/>
-    </row>
-    <row r="58" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="1"/>
-      <c r="B58" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C58" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="D58" s="35"/>
-      <c r="E58" s="35"/>
-      <c r="F58" s="36"/>
-      <c r="G58" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="H58" s="35"/>
-      <c r="I58" s="35"/>
-      <c r="J58" s="35"/>
-      <c r="K58" s="35"/>
-      <c r="L58" s="36"/>
-      <c r="M58" s="1"/>
-    </row>
-    <row r="59" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="1"/>
-      <c r="B59" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="C59" s="26"/>
-      <c r="D59" s="26"/>
-      <c r="E59" s="26"/>
-      <c r="F59" s="26"/>
-      <c r="G59" s="26"/>
-      <c r="H59" s="26"/>
-      <c r="I59" s="26"/>
-      <c r="J59" s="26"/>
-      <c r="K59" s="26"/>
-      <c r="L59" s="27"/>
-      <c r="M59" s="1"/>
-    </row>
-    <row r="60" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="1"/>
-      <c r="B60" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="C60" s="38"/>
-      <c r="D60" s="38"/>
-      <c r="E60" s="38"/>
-      <c r="F60" s="39"/>
-      <c r="G60" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="H60" s="41"/>
-      <c r="I60" s="41"/>
-      <c r="J60" s="41"/>
-      <c r="K60" s="41"/>
-      <c r="L60" s="42"/>
-      <c r="M60" s="1"/>
-    </row>
-    <row r="61" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A61" s="1"/>
-      <c r="B61" s="43"/>
-      <c r="C61" s="44"/>
-      <c r="D61" s="44"/>
-      <c r="E61" s="44"/>
-      <c r="F61" s="45"/>
-      <c r="G61" s="43"/>
-      <c r="H61" s="44"/>
-      <c r="I61" s="44"/>
-      <c r="J61" s="44"/>
-      <c r="K61" s="44"/>
-      <c r="L61" s="45"/>
-      <c r="M61" s="1"/>
-    </row>
-    <row r="62" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="1"/>
-      <c r="B62" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C62" s="26"/>
-      <c r="D62" s="26"/>
-      <c r="E62" s="26"/>
-      <c r="F62" s="26"/>
-      <c r="G62" s="26"/>
-      <c r="H62" s="26"/>
-      <c r="I62" s="26"/>
-      <c r="J62" s="26"/>
-      <c r="K62" s="26"/>
-      <c r="L62" s="27"/>
-      <c r="M62" s="1"/>
-    </row>
-    <row r="63" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A63" s="1"/>
-      <c r="B63" s="28"/>
-      <c r="C63" s="29"/>
-      <c r="D63" s="29"/>
-      <c r="E63" s="29"/>
-      <c r="F63" s="29"/>
-      <c r="G63" s="29"/>
-      <c r="H63" s="29"/>
-      <c r="I63" s="29"/>
-      <c r="J63" s="29"/>
-      <c r="K63" s="29"/>
-      <c r="L63" s="30"/>
-      <c r="M63" s="1"/>
-    </row>
-    <row r="64" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A64" s="1"/>
-      <c r="B64" s="31"/>
-      <c r="C64" s="32"/>
-      <c r="D64" s="32"/>
-      <c r="E64" s="32"/>
-      <c r="F64" s="32"/>
-      <c r="G64" s="32"/>
-      <c r="H64" s="32"/>
-      <c r="I64" s="32"/>
-      <c r="J64" s="32"/>
-      <c r="K64" s="32"/>
-      <c r="L64" s="33"/>
-      <c r="M64" s="1"/>
-    </row>
-    <row r="65" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="L65" s="1"/>
-      <c r="M65" s="1"/>
-    </row>
-    <row r="66" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A66" s="1"/>
-      <c r="M66" s="1"/>
-    </row>
-    <row r="67" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A67" s="1"/>
-      <c r="M67" s="1"/>
-    </row>
-    <row r="68" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="69" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="70" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="71" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="72" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="73" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="74" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="75" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="76" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="77" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="78" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="79" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="80" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="81" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="82" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="83" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="84" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="85" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="86" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="57" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="58" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="59" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="60" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="61" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="62" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="63" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="64" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="65" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="66" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="67" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="68" ht="14.5" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="69" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="70" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="71" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="72" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="73" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="74" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="75" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="76" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="77" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="78" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="79" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="80" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="81" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="82" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="83" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="84" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="85" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="86" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="87">
-    <mergeCell ref="H40:H54"/>
+  <mergeCells count="82">
     <mergeCell ref="B2:F5"/>
     <mergeCell ref="G2:L5"/>
     <mergeCell ref="B6:L6"/>
@@ -3275,45 +3202,41 @@
     <mergeCell ref="K40:L40"/>
     <mergeCell ref="K41:L41"/>
     <mergeCell ref="K42:L42"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="C55:F55"/>
-    <mergeCell ref="G55:L55"/>
-    <mergeCell ref="C56:F56"/>
-    <mergeCell ref="G56:L56"/>
-    <mergeCell ref="C57:F57"/>
-    <mergeCell ref="G57:L57"/>
-    <mergeCell ref="B62:L62"/>
-    <mergeCell ref="B63:L64"/>
-    <mergeCell ref="C58:F58"/>
-    <mergeCell ref="G58:L58"/>
-    <mergeCell ref="B59:L59"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="G60:L60"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="G61:L61"/>
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="G44:L44"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="G45:L45"/>
+    <mergeCell ref="C46:F46"/>
+    <mergeCell ref="G46:L46"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="B52:L53"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="G47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="G49:L49"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="G50:L50"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="C8:L8">
     <cfRule type="expression" priority="30" stopIfTrue="1">
       <formula>LEN($C$8)=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="31" stopIfTrue="1">
       <formula>LEN(C8)&lt;9</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="32" stopIfTrue="1">
       <formula>LEN(C8)&gt;9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:F16 B19:L23 B26:L30">
-    <cfRule type="expression" dxfId="14" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="29" stopIfTrue="1">
       <formula>LEN(B12)&gt;32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:F18">
-    <cfRule type="expression" dxfId="13" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="27" stopIfTrue="1">
       <formula>LEN($B$18)&gt;32</formula>
     </cfRule>
     <cfRule type="expression" priority="28" stopIfTrue="1">
@@ -3324,12 +3247,12 @@
     <cfRule type="expression" priority="25" stopIfTrue="1">
       <formula>LEN($G$18)=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="26" stopIfTrue="1">
       <formula>LEN($B$11)&gt;32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:F25">
-    <cfRule type="expression" dxfId="11" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="23" stopIfTrue="1">
       <formula>LEN($B$25)&gt;32</formula>
     </cfRule>
     <cfRule type="expression" priority="24" stopIfTrue="1">
@@ -3340,23 +3263,15 @@
     <cfRule type="expression" priority="21" stopIfTrue="1">
       <formula>LEN($G$25)=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="22" stopIfTrue="1">
       <formula>LEN($G$25)&gt;32</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F41:F43 F50:F54 F46:F47">
-    <cfRule type="expression" priority="17" stopIfTrue="1">
-      <formula>LEN(F41)&gt;0</formula>
+  <conditionalFormatting sqref="C45:F45">
+    <cfRule type="expression" priority="15" stopIfTrue="1">
+      <formula>LEN(C45)&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="18" stopIfTrue="1">
-      <formula>LEN(B41)&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56:F56">
-    <cfRule type="expression" priority="15" stopIfTrue="1">
-      <formula>LEN(C56)&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="16" stopIfTrue="1">
       <formula>LEN($C$8)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3364,7 +3279,7 @@
     <cfRule type="expression" priority="9" stopIfTrue="1">
       <formula>LEN($B$11)=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="10" stopIfTrue="1">
       <formula>LEN($B$11)&gt;32</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3372,7 +3287,7 @@
     <cfRule type="expression" priority="7" stopIfTrue="1">
       <formula>LEN($B$18)=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="8" stopIfTrue="1">
       <formula>LEN($B$11)&gt;32</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3380,28 +3295,12 @@
     <cfRule type="expression" priority="5" stopIfTrue="1">
       <formula>LEN($C$9)&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="6" stopIfTrue="1">
       <formula>LEN($C$8)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F48:F49">
-    <cfRule type="expression" priority="3" stopIfTrue="1">
-      <formula>LEN(F48)&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
-      <formula>LEN(B48)&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F44:F45">
-    <cfRule type="expression" priority="1" stopIfTrue="1">
-      <formula>LEN(F44)&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
-      <formula>LEN(B44)&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" sqref="C56:F58" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="C45:F47" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Payterm</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="32 chars per line" sqref="B12:F16 B18:F23 B25:L30" xr:uid="{00000000-0002-0000-0000-000001000000}"/>

</xml_diff>

<commit_message>
Added declarationNumber to B/L
</commit_message>
<xml_diff>
--- a/AmbRcnTradeServer/ExcelTemplates/Maersk Draft BL Template BL.xlsx
+++ b/AmbRcnTradeServer/ExcelTemplates/Maersk Draft BL Template BL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Visual Studio\AmbRcnTrade\AmbRcnTradeServer\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF473B2A-D585-43BA-9973-13D37D9B4709}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42301A74-D81D-49D5-96A0-91316D77B711}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="10680" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
   <si>
     <t>Shipping Instruction submitter (who should Safmarine Line contact in case of  any queries to this document)</t>
   </si>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t>Container.Rows</t>
+  </si>
+  <si>
+    <t>Container No</t>
   </si>
 </sst>
 </file>
@@ -994,6 +997,264 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1057,18 +1318,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1077,252 +1326,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1742,8 +1745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41:L41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -1779,79 +1782,79 @@
     </row>
     <row r="2" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="53"/>
+      <c r="B2" s="117"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="127"/>
+      <c r="I2" s="127"/>
+      <c r="J2" s="127"/>
+      <c r="K2" s="127"/>
+      <c r="L2" s="128"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="56"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="121"/>
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="130"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="130"/>
+      <c r="K3" s="130"/>
+      <c r="L3" s="131"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="56"/>
+      <c r="B4" s="120"/>
+      <c r="C4" s="121"/>
+      <c r="D4" s="121"/>
+      <c r="E4" s="121"/>
+      <c r="F4" s="122"/>
+      <c r="G4" s="129"/>
+      <c r="H4" s="130"/>
+      <c r="I4" s="130"/>
+      <c r="J4" s="130"/>
+      <c r="K4" s="130"/>
+      <c r="L4" s="131"/>
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="59"/>
+      <c r="B5" s="123"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
+      <c r="E5" s="124"/>
+      <c r="F5" s="125"/>
+      <c r="G5" s="132"/>
+      <c r="H5" s="133"/>
+      <c r="I5" s="133"/>
+      <c r="J5" s="133"/>
+      <c r="K5" s="133"/>
+      <c r="L5" s="134"/>
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1"/>
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="61"/>
-      <c r="L6" s="62"/>
+      <c r="C6" s="136"/>
+      <c r="D6" s="136"/>
+      <c r="E6" s="136"/>
+      <c r="F6" s="136"/>
+      <c r="G6" s="136"/>
+      <c r="H6" s="136"/>
+      <c r="I6" s="136"/>
+      <c r="J6" s="136"/>
+      <c r="K6" s="136"/>
+      <c r="L6" s="137"/>
       <c r="M6" s="1"/>
       <c r="N6" s="2"/>
     </row>
@@ -1860,20 +1863,20 @@
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="65"/>
+      <c r="D7" s="112"/>
+      <c r="E7" s="112"/>
+      <c r="F7" s="113"/>
       <c r="G7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="66"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="67"/>
-      <c r="L7" s="68"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="139"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="139"/>
+      <c r="L7" s="140"/>
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1881,18 +1884,18 @@
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="111" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="64"/>
-      <c r="L8" s="65"/>
+      <c r="D8" s="112"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="112"/>
+      <c r="G8" s="112"/>
+      <c r="H8" s="112"/>
+      <c r="I8" s="112"/>
+      <c r="J8" s="112"/>
+      <c r="K8" s="112"/>
+      <c r="L8" s="113"/>
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1900,196 +1903,196 @@
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="111" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="65"/>
+      <c r="D9" s="112"/>
+      <c r="E9" s="112"/>
+      <c r="F9" s="113"/>
       <c r="G9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="63">
+      <c r="H9" s="111">
         <v>3</v>
       </c>
-      <c r="I9" s="64"/>
-      <c r="J9" s="64"/>
-      <c r="K9" s="64"/>
-      <c r="L9" s="65"/>
+      <c r="I9" s="112"/>
+      <c r="J9" s="112"/>
+      <c r="K9" s="112"/>
+      <c r="L9" s="113"/>
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="1"/>
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="106" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="70"/>
-      <c r="D10" s="70"/>
-      <c r="E10" s="70"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="72" t="s">
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="107"/>
+      <c r="G10" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="74"/>
+      <c r="H10" s="115"/>
+      <c r="I10" s="115"/>
+      <c r="J10" s="115"/>
+      <c r="K10" s="115"/>
+      <c r="L10" s="116"/>
       <c r="M10" s="6"/>
       <c r="N10" s="7"/>
     </row>
     <row r="11" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="76"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="77"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="92"/>
+      <c r="F11" s="93"/>
       <c r="G11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="78" t="s">
+      <c r="H11" s="108" t="s">
         <v>55</v>
       </c>
-      <c r="I11" s="79"/>
-      <c r="J11" s="79"/>
-      <c r="K11" s="79"/>
-      <c r="L11" s="80"/>
+      <c r="I11" s="109"/>
+      <c r="J11" s="109"/>
+      <c r="K11" s="109"/>
+      <c r="L11" s="110"/>
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
-      <c r="B12" s="81" t="s">
+      <c r="B12" s="80" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="82"/>
-      <c r="D12" s="82"/>
-      <c r="E12" s="82"/>
-      <c r="F12" s="83"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="81"/>
       <c r="G12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="84" t="s">
+      <c r="H12" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="I12" s="82"/>
-      <c r="J12" s="82"/>
-      <c r="K12" s="82"/>
-      <c r="L12" s="83"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="81"/>
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="83"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="81"/>
       <c r="G13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="84" t="s">
+      <c r="H13" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="I13" s="82"/>
-      <c r="J13" s="82"/>
-      <c r="K13" s="82"/>
-      <c r="L13" s="83"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="81"/>
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
-      <c r="B14" s="81" t="s">
+      <c r="B14" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="82"/>
-      <c r="D14" s="82"/>
-      <c r="E14" s="82"/>
-      <c r="F14" s="83"/>
-      <c r="G14" s="85" t="s">
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
-      <c r="J14" s="86"/>
-      <c r="K14" s="86"/>
-      <c r="L14" s="87"/>
+      <c r="H14" s="98"/>
+      <c r="I14" s="98"/>
+      <c r="J14" s="98"/>
+      <c r="K14" s="98"/>
+      <c r="L14" s="99"/>
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="80" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="82"/>
-      <c r="D15" s="82"/>
-      <c r="E15" s="82"/>
-      <c r="F15" s="83"/>
-      <c r="G15" s="88"/>
-      <c r="H15" s="89"/>
-      <c r="I15" s="89"/>
-      <c r="J15" s="89"/>
-      <c r="K15" s="89"/>
-      <c r="L15" s="90"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="100"/>
+      <c r="H15" s="101"/>
+      <c r="I15" s="101"/>
+      <c r="J15" s="101"/>
+      <c r="K15" s="101"/>
+      <c r="L15" s="102"/>
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="1"/>
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="80" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="82"/>
-      <c r="D16" s="82"/>
-      <c r="E16" s="82"/>
-      <c r="F16" s="83"/>
-      <c r="G16" s="91"/>
-      <c r="H16" s="92"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="92"/>
-      <c r="L16" s="93"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="81"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="104"/>
+      <c r="I16" s="104"/>
+      <c r="J16" s="104"/>
+      <c r="K16" s="104"/>
+      <c r="L16" s="105"/>
       <c r="M16" s="1"/>
     </row>
     <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1"/>
-      <c r="B17" s="69" t="s">
+      <c r="B17" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="69" t="s">
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="89"/>
+      <c r="F17" s="107"/>
+      <c r="G17" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="70"/>
-      <c r="I17" s="70"/>
-      <c r="J17" s="70"/>
-      <c r="K17" s="70"/>
-      <c r="L17" s="71"/>
+      <c r="H17" s="89"/>
+      <c r="I17" s="89"/>
+      <c r="J17" s="89"/>
+      <c r="K17" s="89"/>
+      <c r="L17" s="107"/>
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
-      <c r="B18" s="75" t="s">
+      <c r="B18" s="91" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="76"/>
-      <c r="F18" s="77"/>
-      <c r="G18" s="75" t="s">
+      <c r="C18" s="92"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="93"/>
+      <c r="G18" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="H18" s="76"/>
-      <c r="I18" s="76"/>
-      <c r="J18" s="76"/>
-      <c r="K18" s="76"/>
-      <c r="L18" s="77"/>
+      <c r="H18" s="92"/>
+      <c r="I18" s="92"/>
+      <c r="J18" s="92"/>
+      <c r="K18" s="92"/>
+      <c r="L18" s="93"/>
       <c r="M18" s="1"/>
     </row>
     <row r="19" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
@@ -2101,14 +2104,14 @@
       <c r="D19" s="95"/>
       <c r="E19" s="95"/>
       <c r="F19" s="96"/>
-      <c r="G19" s="81" t="s">
+      <c r="G19" s="80" t="s">
         <v>57</v>
       </c>
-      <c r="H19" s="82"/>
-      <c r="I19" s="82"/>
-      <c r="J19" s="82"/>
-      <c r="K19" s="82"/>
-      <c r="L19" s="83"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="81"/>
       <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
@@ -2120,14 +2123,14 @@
       <c r="D20" s="95"/>
       <c r="E20" s="95"/>
       <c r="F20" s="96"/>
-      <c r="G20" s="81" t="s">
+      <c r="G20" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="82"/>
-      <c r="K20" s="82"/>
-      <c r="L20" s="83"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="81"/>
       <c r="M20" s="1"/>
     </row>
     <row r="21" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
@@ -2139,14 +2142,14 @@
       <c r="D21" s="95"/>
       <c r="E21" s="95"/>
       <c r="F21" s="96"/>
-      <c r="G21" s="81" t="s">
+      <c r="G21" s="80" t="s">
         <v>59</v>
       </c>
-      <c r="H21" s="82"/>
-      <c r="I21" s="82"/>
-      <c r="J21" s="82"/>
-      <c r="K21" s="82"/>
-      <c r="L21" s="83"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="81"/>
       <c r="M21" s="1"/>
     </row>
     <row r="22" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
@@ -2158,14 +2161,14 @@
       <c r="D22" s="95"/>
       <c r="E22" s="95"/>
       <c r="F22" s="96"/>
-      <c r="G22" s="81" t="s">
+      <c r="G22" s="80" t="s">
         <v>60</v>
       </c>
-      <c r="H22" s="82"/>
-      <c r="I22" s="82"/>
-      <c r="J22" s="82"/>
-      <c r="K22" s="82"/>
-      <c r="L22" s="83"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="81"/>
       <c r="M22" s="1"/>
     </row>
     <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2177,147 +2180,147 @@
       <c r="D23" s="95"/>
       <c r="E23" s="95"/>
       <c r="F23" s="96"/>
-      <c r="G23" s="81" t="s">
+      <c r="G23" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="H23" s="82"/>
-      <c r="I23" s="82"/>
-      <c r="J23" s="82"/>
-      <c r="K23" s="82"/>
-      <c r="L23" s="83"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="81"/>
       <c r="M23" s="1"/>
     </row>
     <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="1"/>
-      <c r="B24" s="97" t="s">
+      <c r="B24" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="70"/>
-      <c r="D24" s="70"/>
-      <c r="E24" s="70"/>
-      <c r="F24" s="98"/>
-      <c r="G24" s="97" t="s">
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="89"/>
+      <c r="F24" s="90"/>
+      <c r="G24" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="H24" s="70"/>
-      <c r="I24" s="70"/>
-      <c r="J24" s="70"/>
-      <c r="K24" s="70"/>
-      <c r="L24" s="98"/>
+      <c r="H24" s="89"/>
+      <c r="I24" s="89"/>
+      <c r="J24" s="89"/>
+      <c r="K24" s="89"/>
+      <c r="L24" s="90"/>
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
-      <c r="B25" s="75" t="s">
+      <c r="B25" s="91" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="76"/>
-      <c r="D25" s="76"/>
-      <c r="E25" s="76"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="75" t="s">
+      <c r="C25" s="92"/>
+      <c r="D25" s="92"/>
+      <c r="E25" s="92"/>
+      <c r="F25" s="93"/>
+      <c r="G25" s="91" t="s">
         <v>75</v>
       </c>
-      <c r="H25" s="76"/>
-      <c r="I25" s="76"/>
-      <c r="J25" s="76"/>
-      <c r="K25" s="76"/>
-      <c r="L25" s="77"/>
+      <c r="H25" s="92"/>
+      <c r="I25" s="92"/>
+      <c r="J25" s="92"/>
+      <c r="K25" s="92"/>
+      <c r="L25" s="93"/>
       <c r="M25" s="1"/>
     </row>
     <row r="26" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
-      <c r="B26" s="81" t="s">
+      <c r="B26" s="80" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="82"/>
-      <c r="D26" s="82"/>
-      <c r="E26" s="82"/>
-      <c r="F26" s="83"/>
-      <c r="G26" s="81" t="s">
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="81"/>
+      <c r="G26" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="H26" s="82"/>
-      <c r="I26" s="82"/>
-      <c r="J26" s="82"/>
-      <c r="K26" s="82"/>
-      <c r="L26" s="83"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="81"/>
       <c r="M26" s="1"/>
     </row>
     <row r="27" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
-      <c r="B27" s="81" t="s">
+      <c r="B27" s="80" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="82"/>
-      <c r="D27" s="82"/>
-      <c r="E27" s="82"/>
-      <c r="F27" s="83"/>
-      <c r="G27" s="81" t="s">
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="81"/>
+      <c r="G27" s="80" t="s">
         <v>77</v>
       </c>
-      <c r="H27" s="82"/>
-      <c r="I27" s="82"/>
-      <c r="J27" s="82"/>
-      <c r="K27" s="82"/>
-      <c r="L27" s="83"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="53"/>
+      <c r="K27" s="53"/>
+      <c r="L27" s="81"/>
       <c r="M27" s="1"/>
     </row>
     <row r="28" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
-      <c r="B28" s="81" t="s">
+      <c r="B28" s="80" t="s">
         <v>85</v>
       </c>
-      <c r="C28" s="82"/>
-      <c r="D28" s="82"/>
-      <c r="E28" s="82"/>
-      <c r="F28" s="83"/>
-      <c r="G28" s="81" t="s">
+      <c r="C28" s="53"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="81"/>
+      <c r="G28" s="80" t="s">
         <v>78</v>
       </c>
-      <c r="H28" s="82"/>
-      <c r="I28" s="82"/>
-      <c r="J28" s="82"/>
-      <c r="K28" s="82"/>
-      <c r="L28" s="83"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="81"/>
       <c r="M28" s="1"/>
     </row>
     <row r="29" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
-      <c r="B29" s="81" t="s">
+      <c r="B29" s="80" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="82"/>
-      <c r="D29" s="82"/>
-      <c r="E29" s="82"/>
-      <c r="F29" s="83"/>
-      <c r="G29" s="81" t="s">
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="81"/>
+      <c r="G29" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="H29" s="82"/>
-      <c r="I29" s="82"/>
-      <c r="J29" s="82"/>
-      <c r="K29" s="82"/>
-      <c r="L29" s="83"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="53"/>
+      <c r="L29" s="81"/>
       <c r="M29" s="1"/>
     </row>
     <row r="30" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
-      <c r="B30" s="81" t="s">
+      <c r="B30" s="80" t="s">
         <v>87</v>
       </c>
-      <c r="C30" s="82"/>
-      <c r="D30" s="82"/>
-      <c r="E30" s="82"/>
-      <c r="F30" s="83"/>
-      <c r="G30" s="81" t="s">
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="81"/>
+      <c r="G30" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="H30" s="82"/>
-      <c r="I30" s="82"/>
-      <c r="J30" s="82"/>
-      <c r="K30" s="82"/>
-      <c r="L30" s="83"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="53"/>
+      <c r="K30" s="53"/>
+      <c r="L30" s="81"/>
       <c r="M30" s="1"/>
     </row>
     <row r="31" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
@@ -2325,58 +2328,58 @@
       <c r="B31" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="84" t="s">
+      <c r="C31" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="82"/>
-      <c r="E31" s="82"/>
-      <c r="F31" s="99"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="54"/>
       <c r="G31" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H31" s="84" t="s">
+      <c r="H31" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="I31" s="82"/>
-      <c r="J31" s="82"/>
-      <c r="K31" s="82"/>
-      <c r="L31" s="99"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="53"/>
+      <c r="K31" s="53"/>
+      <c r="L31" s="54"/>
       <c r="M31" s="1"/>
     </row>
     <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
-      <c r="B32" s="100" t="s">
+      <c r="B32" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="101"/>
-      <c r="D32" s="101"/>
-      <c r="E32" s="101"/>
-      <c r="F32" s="102"/>
-      <c r="G32" s="103" t="s">
+      <c r="C32" s="83"/>
+      <c r="D32" s="83"/>
+      <c r="E32" s="83"/>
+      <c r="F32" s="84"/>
+      <c r="G32" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="H32" s="104"/>
-      <c r="I32" s="104"/>
-      <c r="J32" s="104"/>
-      <c r="K32" s="104"/>
-      <c r="L32" s="105"/>
+      <c r="H32" s="86"/>
+      <c r="I32" s="86"/>
+      <c r="J32" s="86"/>
+      <c r="K32" s="86"/>
+      <c r="L32" s="87"/>
       <c r="M32" s="1"/>
     </row>
     <row r="33" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
-      <c r="B33" s="106"/>
-      <c r="C33" s="107"/>
-      <c r="D33" s="107"/>
-      <c r="E33" s="107"/>
-      <c r="F33" s="108"/>
-      <c r="G33" s="106" t="s">
+      <c r="B33" s="77"/>
+      <c r="C33" s="78"/>
+      <c r="D33" s="78"/>
+      <c r="E33" s="78"/>
+      <c r="F33" s="79"/>
+      <c r="G33" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="H33" s="107"/>
-      <c r="I33" s="107"/>
-      <c r="J33" s="107"/>
-      <c r="K33" s="107"/>
-      <c r="L33" s="108"/>
+      <c r="H33" s="78"/>
+      <c r="I33" s="78"/>
+      <c r="J33" s="78"/>
+      <c r="K33" s="78"/>
+      <c r="L33" s="79"/>
       <c r="M33" s="1"/>
     </row>
     <row r="34" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2384,20 +2387,20 @@
       <c r="B34" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="109" t="s">
+      <c r="C34" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="110"/>
-      <c r="E34" s="110"/>
-      <c r="F34" s="111"/>
-      <c r="G34" s="112" t="s">
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="H34" s="113"/>
-      <c r="I34" s="113"/>
-      <c r="J34" s="113"/>
-      <c r="K34" s="113"/>
-      <c r="L34" s="114"/>
+      <c r="H34" s="72"/>
+      <c r="I34" s="72"/>
+      <c r="J34" s="72"/>
+      <c r="K34" s="72"/>
+      <c r="L34" s="73"/>
       <c r="M34" s="1"/>
     </row>
     <row r="35" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
@@ -2405,18 +2408,18 @@
       <c r="B35" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="106" t="s">
+      <c r="C35" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="D35" s="107"/>
-      <c r="E35" s="107"/>
-      <c r="F35" s="108"/>
-      <c r="G35" s="84"/>
-      <c r="H35" s="82"/>
-      <c r="I35" s="82"/>
-      <c r="J35" s="82"/>
-      <c r="K35" s="82"/>
-      <c r="L35" s="99"/>
+      <c r="D35" s="78"/>
+      <c r="E35" s="78"/>
+      <c r="F35" s="79"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="53"/>
+      <c r="J35" s="53"/>
+      <c r="K35" s="53"/>
+      <c r="L35" s="54"/>
       <c r="M35" s="1"/>
     </row>
     <row r="36" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2424,20 +2427,20 @@
       <c r="B36" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="109" t="s">
+      <c r="C36" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="110"/>
-      <c r="E36" s="110"/>
-      <c r="F36" s="111"/>
-      <c r="G36" s="112" t="s">
+      <c r="D36" s="69"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="H36" s="113"/>
-      <c r="I36" s="113"/>
-      <c r="J36" s="113"/>
-      <c r="K36" s="113"/>
-      <c r="L36" s="114"/>
+      <c r="H36" s="72"/>
+      <c r="I36" s="72"/>
+      <c r="J36" s="72"/>
+      <c r="K36" s="72"/>
+      <c r="L36" s="73"/>
       <c r="M36" s="1"/>
     </row>
     <row r="37" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
@@ -2445,40 +2448,42 @@
       <c r="B37" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="84" t="s">
+      <c r="C37" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="D37" s="82"/>
-      <c r="E37" s="82"/>
-      <c r="F37" s="99"/>
-      <c r="G37" s="84"/>
-      <c r="H37" s="82"/>
-      <c r="I37" s="82"/>
-      <c r="J37" s="82"/>
-      <c r="K37" s="82"/>
-      <c r="L37" s="99"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="54"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="53"/>
+      <c r="K37" s="53"/>
+      <c r="L37" s="54"/>
       <c r="M37" s="1"/>
     </row>
     <row r="38" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
-      <c r="B38" s="115" t="s">
+      <c r="B38" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="116"/>
-      <c r="D38" s="116"/>
-      <c r="E38" s="116"/>
-      <c r="F38" s="116"/>
-      <c r="G38" s="116"/>
-      <c r="H38" s="116"/>
-      <c r="I38" s="116"/>
-      <c r="J38" s="116"/>
-      <c r="K38" s="116"/>
-      <c r="L38" s="117"/>
+      <c r="C38" s="75"/>
+      <c r="D38" s="75"/>
+      <c r="E38" s="75"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="75"/>
+      <c r="H38" s="75"/>
+      <c r="I38" s="75"/>
+      <c r="J38" s="75"/>
+      <c r="K38" s="75"/>
+      <c r="L38" s="76"/>
       <c r="M38" s="1"/>
     </row>
     <row r="39" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
-      <c r="B39" s="25"/>
+      <c r="B39" s="15" t="s">
+        <v>103</v>
+      </c>
       <c r="C39" s="15" t="s">
         <v>28</v>
       </c>
@@ -2503,10 +2508,10 @@
       <c r="J39" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="K39" s="118" t="s">
+      <c r="K39" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="L39" s="119"/>
+      <c r="L39" s="60"/>
       <c r="M39" s="1"/>
     </row>
     <row r="40" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2524,10 +2529,10 @@
       <c r="H40" s="25"/>
       <c r="I40" s="26"/>
       <c r="J40" s="26"/>
-      <c r="K40" s="120">
+      <c r="K40" s="61">
         <v>999</v>
       </c>
-      <c r="L40" s="120"/>
+      <c r="L40" s="61"/>
       <c r="M40" s="1"/>
     </row>
     <row r="41" spans="1:13" ht="67" customHeight="1" x14ac:dyDescent="0.35">
@@ -2551,8 +2556,8 @@
       <c r="J41" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="K41" s="121"/>
-      <c r="L41" s="122"/>
+      <c r="K41" s="62"/>
+      <c r="L41" s="63"/>
       <c r="M41" s="1"/>
     </row>
     <row r="42" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
@@ -2568,8 +2573,8 @@
       <c r="H42" s="29"/>
       <c r="I42" s="30"/>
       <c r="J42" s="30"/>
-      <c r="K42" s="123"/>
-      <c r="L42" s="124"/>
+      <c r="K42" s="64"/>
+      <c r="L42" s="65"/>
       <c r="M42" s="1"/>
     </row>
     <row r="43" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
@@ -2594,20 +2599,20 @@
       <c r="B44" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="125" t="s">
+      <c r="C44" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="D44" s="125"/>
-      <c r="E44" s="125"/>
-      <c r="F44" s="125"/>
-      <c r="G44" s="126" t="s">
+      <c r="D44" s="66"/>
+      <c r="E44" s="66"/>
+      <c r="F44" s="66"/>
+      <c r="G44" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="H44" s="126"/>
-      <c r="I44" s="126"/>
-      <c r="J44" s="126"/>
-      <c r="K44" s="126"/>
-      <c r="L44" s="126"/>
+      <c r="H44" s="67"/>
+      <c r="I44" s="67"/>
+      <c r="J44" s="67"/>
+      <c r="K44" s="67"/>
+      <c r="L44" s="67"/>
       <c r="M44" s="1"/>
     </row>
     <row r="45" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
@@ -2615,20 +2620,20 @@
       <c r="B45" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="127" t="s">
+      <c r="C45" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="D45" s="127"/>
-      <c r="E45" s="127"/>
-      <c r="F45" s="127"/>
-      <c r="G45" s="127" t="s">
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="55"/>
+      <c r="G45" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="H45" s="127"/>
-      <c r="I45" s="127"/>
-      <c r="J45" s="127"/>
-      <c r="K45" s="127"/>
-      <c r="L45" s="127"/>
+      <c r="H45" s="55"/>
+      <c r="I45" s="55"/>
+      <c r="J45" s="55"/>
+      <c r="K45" s="55"/>
+      <c r="L45" s="55"/>
       <c r="M45" s="1"/>
     </row>
     <row r="46" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
@@ -2636,20 +2641,20 @@
       <c r="B46" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="128" t="s">
+      <c r="C46" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="D46" s="128"/>
-      <c r="E46" s="128"/>
-      <c r="F46" s="128"/>
-      <c r="G46" s="128" t="s">
+      <c r="D46" s="48"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="H46" s="128"/>
-      <c r="I46" s="128"/>
-      <c r="J46" s="128"/>
-      <c r="K46" s="128"/>
-      <c r="L46" s="128"/>
+      <c r="H46" s="48"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
+      <c r="K46" s="48"/>
+      <c r="L46" s="48"/>
       <c r="M46" s="1"/>
     </row>
     <row r="47" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
@@ -2657,118 +2662,118 @@
       <c r="B47" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C47" s="128" t="s">
+      <c r="C47" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="D47" s="128"/>
-      <c r="E47" s="128"/>
-      <c r="F47" s="128"/>
-      <c r="G47" s="128" t="s">
+      <c r="D47" s="48"/>
+      <c r="E47" s="48"/>
+      <c r="F47" s="48"/>
+      <c r="G47" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="H47" s="128"/>
-      <c r="I47" s="128"/>
-      <c r="J47" s="128"/>
-      <c r="K47" s="128"/>
-      <c r="L47" s="128"/>
+      <c r="H47" s="48"/>
+      <c r="I47" s="48"/>
+      <c r="J47" s="48"/>
+      <c r="K47" s="48"/>
+      <c r="L47" s="48"/>
       <c r="M47" s="1"/>
     </row>
     <row r="48" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
-      <c r="B48" s="138" t="s">
+      <c r="B48" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="C48" s="138"/>
-      <c r="D48" s="138"/>
-      <c r="E48" s="138"/>
-      <c r="F48" s="138"/>
-      <c r="G48" s="138"/>
-      <c r="H48" s="138"/>
-      <c r="I48" s="138"/>
-      <c r="J48" s="138"/>
-      <c r="K48" s="138"/>
-      <c r="L48" s="138"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="49"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="49"/>
+      <c r="H48" s="49"/>
+      <c r="I48" s="49"/>
+      <c r="J48" s="49"/>
+      <c r="K48" s="49"/>
+      <c r="L48" s="49"/>
       <c r="M48" s="1"/>
     </row>
     <row r="49" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1"/>
-      <c r="B49" s="139" t="s">
+      <c r="B49" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="C49" s="139"/>
-      <c r="D49" s="139"/>
-      <c r="E49" s="139"/>
-      <c r="F49" s="139"/>
-      <c r="G49" s="140" t="s">
+      <c r="C49" s="50"/>
+      <c r="D49" s="50"/>
+      <c r="E49" s="50"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="H49" s="140"/>
-      <c r="I49" s="140"/>
-      <c r="J49" s="140"/>
-      <c r="K49" s="140"/>
-      <c r="L49" s="140"/>
+      <c r="H49" s="51"/>
+      <c r="I49" s="51"/>
+      <c r="J49" s="51"/>
+      <c r="K49" s="51"/>
+      <c r="L49" s="51"/>
       <c r="M49" s="1"/>
     </row>
     <row r="50" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A50" s="1"/>
-      <c r="B50" s="84"/>
-      <c r="C50" s="82"/>
-      <c r="D50" s="82"/>
-      <c r="E50" s="82"/>
-      <c r="F50" s="99"/>
-      <c r="G50" s="84"/>
-      <c r="H50" s="82"/>
-      <c r="I50" s="82"/>
-      <c r="J50" s="82"/>
-      <c r="K50" s="82"/>
-      <c r="L50" s="99"/>
+      <c r="B50" s="52"/>
+      <c r="C50" s="53"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="54"/>
+      <c r="G50" s="52"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="53"/>
+      <c r="J50" s="53"/>
+      <c r="K50" s="53"/>
+      <c r="L50" s="54"/>
       <c r="M50" s="1"/>
     </row>
     <row r="51" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
-      <c r="B51" s="129" t="s">
+      <c r="B51" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="C51" s="130"/>
-      <c r="D51" s="130"/>
-      <c r="E51" s="130"/>
-      <c r="F51" s="130"/>
-      <c r="G51" s="130"/>
-      <c r="H51" s="130"/>
-      <c r="I51" s="130"/>
-      <c r="J51" s="130"/>
-      <c r="K51" s="130"/>
-      <c r="L51" s="131"/>
+      <c r="C51" s="57"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="57"/>
+      <c r="H51" s="57"/>
+      <c r="I51" s="57"/>
+      <c r="J51" s="57"/>
+      <c r="K51" s="57"/>
+      <c r="L51" s="58"/>
       <c r="M51" s="1"/>
     </row>
     <row r="52" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A52" s="1"/>
-      <c r="B52" s="132"/>
-      <c r="C52" s="133"/>
-      <c r="D52" s="133"/>
-      <c r="E52" s="133"/>
-      <c r="F52" s="133"/>
-      <c r="G52" s="133"/>
-      <c r="H52" s="133"/>
-      <c r="I52" s="133"/>
-      <c r="J52" s="133"/>
-      <c r="K52" s="133"/>
-      <c r="L52" s="134"/>
+      <c r="B52" s="42"/>
+      <c r="C52" s="43"/>
+      <c r="D52" s="43"/>
+      <c r="E52" s="43"/>
+      <c r="F52" s="43"/>
+      <c r="G52" s="43"/>
+      <c r="H52" s="43"/>
+      <c r="I52" s="43"/>
+      <c r="J52" s="43"/>
+      <c r="K52" s="43"/>
+      <c r="L52" s="44"/>
       <c r="M52" s="1"/>
     </row>
     <row r="53" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A53" s="1"/>
-      <c r="B53" s="135"/>
-      <c r="C53" s="136"/>
-      <c r="D53" s="136"/>
-      <c r="E53" s="136"/>
-      <c r="F53" s="136"/>
-      <c r="G53" s="136"/>
-      <c r="H53" s="136"/>
-      <c r="I53" s="136"/>
-      <c r="J53" s="136"/>
-      <c r="K53" s="136"/>
-      <c r="L53" s="137"/>
+      <c r="B53" s="45"/>
+      <c r="C53" s="46"/>
+      <c r="D53" s="46"/>
+      <c r="E53" s="46"/>
+      <c r="F53" s="46"/>
+      <c r="G53" s="46"/>
+      <c r="H53" s="46"/>
+      <c r="I53" s="46"/>
+      <c r="J53" s="46"/>
+      <c r="K53" s="46"/>
+      <c r="L53" s="47"/>
       <c r="M53" s="1"/>
     </row>
     <row r="54" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
@@ -2815,6 +2820,80 @@
     <row r="75" ht="14.5" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="82">
+    <mergeCell ref="B2:F5"/>
+    <mergeCell ref="G2:L5"/>
+    <mergeCell ref="B6:L6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="H9:L9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="G10:L10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="G14:L16"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="G17:L17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="G18:L18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="G19:L19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="G20:L20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="G21:L21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="G22:L22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="G23:L23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="G24:L24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="G25:L25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="G26:L26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="G27:L27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="G28:L28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="G29:L29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="G30:L30"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="G32:L32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="G33:L33"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="G34:L34"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="G35:L35"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="G36:L36"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="G37:L37"/>
+    <mergeCell ref="B38:L38"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="G44:L44"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="G45:L45"/>
+    <mergeCell ref="C46:F46"/>
+    <mergeCell ref="G46:L46"/>
+    <mergeCell ref="B51:L51"/>
     <mergeCell ref="B52:L53"/>
     <mergeCell ref="C47:F47"/>
     <mergeCell ref="G47:L47"/>
@@ -2823,80 +2902,6 @@
     <mergeCell ref="G49:L49"/>
     <mergeCell ref="B50:F50"/>
     <mergeCell ref="G50:L50"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="G45:L45"/>
-    <mergeCell ref="C46:F46"/>
-    <mergeCell ref="G46:L46"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="K41:L41"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="C44:F44"/>
-    <mergeCell ref="G44:L44"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="G36:L36"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="G37:L37"/>
-    <mergeCell ref="B38:L38"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="G33:L33"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="G34:L34"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="G35:L35"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="G30:L30"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="G32:L32"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="G27:L27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="G28:L28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="G29:L29"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="G24:L24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="G25:L25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="G26:L26"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="G21:L21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="G22:L22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="G23:L23"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="G18:L18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="G19:L19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="G20:L20"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="G14:L16"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="G17:L17"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="H9:L9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="G10:L10"/>
-    <mergeCell ref="B2:F5"/>
-    <mergeCell ref="G2:L5"/>
-    <mergeCell ref="B6:L6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="H7:L7"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="C8:L8">
@@ -3001,12 +3006,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3187,15 +3189,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33C41FCB-279C-450E-81D1-E323F4CA622F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3942C816-0066-4A4E-9CBE-620D36D4718B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3220,10 +3226,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3942C816-0066-4A4E-9CBE-620D36D4718B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33C41FCB-279C-450E-81D1-E323F4CA622F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>